<commit_message>
new file:   models/prophet_model.joblib modified:   models/sarima_model.joblib modified:   notebooks/store_sales_forecast.ipynb modified:   outputs/SARIMA_sales_forecast.xlsx new file:   outputs/prophet_sales_forecast.xlsx
</commit_message>
<xml_diff>
--- a/outputs/SARIMA_sales_forecast.xlsx
+++ b/outputs/SARIMA_sales_forecast.xlsx
@@ -461,7 +461,7 @@
         <v>42736</v>
       </c>
       <c r="B2" t="n">
-        <v>1154739.40406685</v>
+        <v>1153682.926250385</v>
       </c>
       <c r="C2" t="n">
         <v>12082.500997</v>
@@ -472,7 +472,7 @@
         <v>42737</v>
       </c>
       <c r="B3" t="n">
-        <v>1247068.205602113</v>
+        <v>1246758.041321444</v>
       </c>
       <c r="C3" t="n">
         <v>1402306.370834</v>
@@ -483,7 +483,7 @@
         <v>42738</v>
       </c>
       <c r="B4" t="n">
-        <v>948657.1188270287</v>
+        <v>948943.3902764432</v>
       </c>
       <c r="C4" t="n">
         <v>1104377.0798245</v>
@@ -494,7 +494,7 @@
         <v>42739</v>
       </c>
       <c r="B5" t="n">
-        <v>932657.6376031348</v>
+        <v>932933.6798767837</v>
       </c>
       <c r="C5" t="n">
         <v>990093.4637420001</v>
@@ -505,7 +505,7 @@
         <v>42740</v>
       </c>
       <c r="B6" t="n">
-        <v>957099.7955073006</v>
+        <v>957450.9911664735</v>
       </c>
       <c r="C6" t="n">
         <v>777620.9540695</v>
@@ -516,7 +516,7 @@
         <v>42741</v>
       </c>
       <c r="B7" t="n">
-        <v>940935.7667862448</v>
+        <v>941670.5007358722</v>
       </c>
       <c r="C7" t="n">
         <v>839600.237989</v>
@@ -527,7 +527,7 @@
         <v>42742</v>
       </c>
       <c r="B8" t="n">
-        <v>1011480.32916276</v>
+        <v>1012215.840446734</v>
       </c>
       <c r="C8" t="n">
         <v>1103806.298949</v>
@@ -538,7 +538,7 @@
         <v>42743</v>
       </c>
       <c r="B9" t="n">
-        <v>1111698.220564017</v>
+        <v>1112097.080020959</v>
       </c>
       <c r="C9" t="n">
         <v>1192543.750978</v>
@@ -549,7 +549,7 @@
         <v>42744</v>
       </c>
       <c r="B10" t="n">
-        <v>1194143.451489933</v>
+        <v>1194660.925585052</v>
       </c>
       <c r="C10" t="n">
         <v>793724.8969065</v>
@@ -560,7 +560,7 @@
         <v>42745</v>
       </c>
       <c r="B11" t="n">
-        <v>906722.3803387642</v>
+        <v>907489.4978352296</v>
       </c>
       <c r="C11" t="n">
         <v>742635.5692609</v>
@@ -571,7 +571,7 @@
         <v>42746</v>
       </c>
       <c r="B12" t="n">
-        <v>904675.4456655452</v>
+        <v>905531.6284224122</v>
       </c>
       <c r="C12" t="n">
         <v>770742.690065</v>
@@ -582,7 +582,7 @@
         <v>42747</v>
       </c>
       <c r="B13" t="n">
-        <v>935601.1407115174</v>
+        <v>936462.0827977078</v>
       </c>
       <c r="C13" t="n">
         <v>629635.794004</v>
@@ -593,7 +593,7 @@
         <v>42748</v>
       </c>
       <c r="B14" t="n">
-        <v>924496.8898501059</v>
+        <v>925626.0283044118</v>
       </c>
       <c r="C14" t="n">
         <v>768898.9443881999</v>
@@ -604,7 +604,7 @@
         <v>42749</v>
       </c>
       <c r="B15" t="n">
-        <v>999788.3135271958</v>
+        <v>1000879.506205412</v>
       </c>
       <c r="C15" t="n">
         <v>1021050.536226</v>
@@ -615,7 +615,7 @@
         <v>42750</v>
       </c>
       <c r="B16" t="n">
-        <v>1103558.060399439</v>
+        <v>1104283.559591549</v>
       </c>
       <c r="C16" t="n">
         <v>1175725.165838</v>
@@ -626,7 +626,7 @@
         <v>42751</v>
       </c>
       <c r="B17" t="n">
-        <v>1188677.966072439</v>
+        <v>1189486.956149474</v>
       </c>
       <c r="C17" t="n">
         <v>824488.666175</v>
@@ -637,7 +637,7 @@
         <v>42752</v>
       </c>
       <c r="B18" t="n">
-        <v>903400.9036337654</v>
+        <v>904434.459687929</v>
       </c>
       <c r="C18" t="n">
         <v>750836.542952</v>
@@ -648,7 +648,7 @@
         <v>42753</v>
       </c>
       <c r="B19" t="n">
-        <v>903039.6904707593</v>
+        <v>904144.6410523052</v>
       </c>
       <c r="C19" t="n">
         <v>782656.0246723</v>
@@ -659,7 +659,7 @@
         <v>42754</v>
       </c>
       <c r="B20" t="n">
-        <v>935273.9513455532</v>
+        <v>936368.7252986624</v>
       </c>
       <c r="C20" t="n">
         <v>606949.7448793</v>
@@ -670,7 +670,7 @@
         <v>42755</v>
       </c>
       <c r="B21" t="n">
-        <v>925194.6044060206</v>
+        <v>926545.6173989382</v>
       </c>
       <c r="C21" t="n">
         <v>725703.6910875</v>
@@ -681,7 +681,7 @@
         <v>42756</v>
       </c>
       <c r="B22" t="n">
-        <v>1001289.801280616</v>
+        <v>1002593.716005552</v>
       </c>
       <c r="C22" t="n">
         <v>1072721.724905</v>
@@ -692,7 +692,7 @@
         <v>42757</v>
       </c>
       <c r="B23" t="n">
-        <v>1105688.056816709</v>
+        <v>1106619.057411964</v>
       </c>
       <c r="C23" t="n">
         <v>1148214.358454</v>
@@ -703,7 +703,7 @@
         <v>42758</v>
       </c>
       <c r="B24" t="n">
-        <v>1191299.62601704</v>
+        <v>1192308.385688315</v>
       </c>
       <c r="C24" t="n">
         <v>798133.612125</v>
@@ -714,7 +714,7 @@
         <v>42759</v>
       </c>
       <c r="B25" t="n">
-        <v>906407.4601536677</v>
+        <v>907636.2891775591</v>
       </c>
       <c r="C25" t="n">
         <v>721275.774781</v>
@@ -725,7 +725,7 @@
         <v>42760</v>
       </c>
       <c r="B26" t="n">
-        <v>906347.4661621805</v>
+        <v>907644.1575474866</v>
       </c>
       <c r="C26" t="n">
         <v>744342.5929227</v>
@@ -736,7 +736,7 @@
         <v>42761</v>
       </c>
       <c r="B27" t="n">
-        <v>938817.4304723651</v>
+        <v>940101.1612302719</v>
       </c>
       <c r="C27" t="n">
         <v>576515.5369877</v>
@@ -747,7 +747,7 @@
         <v>42762</v>
       </c>
       <c r="B28" t="n">
-        <v>928922.5441864037</v>
+        <v>930460.3228040917</v>
       </c>
       <c r="C28" t="n">
         <v>722113.958837</v>
@@ -758,7 +758,7 @@
         <v>42763</v>
       </c>
       <c r="B29" t="n">
-        <v>1005162.099734819</v>
+        <v>1006651.056751198</v>
       </c>
       <c r="C29" t="n">
         <v>977850.40585</v>
@@ -769,7 +769,7 @@
         <v>42764</v>
       </c>
       <c r="B30" t="n">
-        <v>1109673.325999645</v>
+        <v>1110788.012683216</v>
       </c>
       <c r="C30" t="n">
         <v>1075166.993043</v>
@@ -780,7 +780,7 @@
         <v>42765</v>
       </c>
       <c r="B31" t="n">
-        <v>1195373.303475743</v>
+        <v>1196564.681937567</v>
       </c>
       <c r="C31" t="n">
         <v>698123.768037</v>
@@ -791,7 +791,7 @@
         <v>42766</v>
       </c>
       <c r="B32" t="n">
-        <v>910550.3244528171</v>
+        <v>911960.932534982</v>
       </c>
       <c r="C32" t="n">
         <v>778222.285925</v>
@@ -802,7 +802,7 @@
         <v>42767</v>
       </c>
       <c r="B33" t="n">
-        <v>910544.4746653857</v>
+        <v>912022.2844107115</v>
       </c>
       <c r="C33" t="n">
         <v>961777.382874</v>
@@ -813,7 +813,7 @@
         <v>42768</v>
       </c>
       <c r="B34" t="n">
-        <v>943056.811074565</v>
+        <v>944521.1403447842</v>
       </c>
       <c r="C34" t="n">
         <v>748882.732615</v>
@@ -824,7 +824,7 @@
         <v>42769</v>
       </c>
       <c r="B35" t="n">
-        <v>933195.0843453137</v>
+        <v>934913.0524748609</v>
       </c>
       <c r="C35" t="n">
         <v>834667.1519293</v>
@@ -835,7 +835,7 @@
         <v>42770</v>
       </c>
       <c r="B36" t="n">
-        <v>1009460.589895571</v>
+        <v>1011129.414646645</v>
       </c>
       <c r="C36" t="n">
         <v>1132788.541413</v>
@@ -846,7 +846,7 @@
         <v>42771</v>
       </c>
       <c r="B37" t="n">
-        <v>1113992.124100535</v>
+        <v>1115286.425368011</v>
       </c>
       <c r="C37" t="n">
         <v>1151987.631095</v>
@@ -857,7 +857,7 @@
         <v>42772</v>
       </c>
       <c r="B38" t="n">
-        <v>1199707.994157363</v>
+        <v>1201078.78804822</v>
       </c>
       <c r="C38" t="n">
         <v>786672.394181</v>
@@ -868,7 +868,7 @@
         <v>42773</v>
       </c>
       <c r="B39" t="n">
-        <v>914897.4523458113</v>
+        <v>916487.3191858631</v>
       </c>
       <c r="C39" t="n">
         <v>739431.213302</v>
@@ -879,7 +879,7 @@
         <v>42774</v>
       </c>
       <c r="B40" t="n">
-        <v>914901.3356670938</v>
+        <v>916558.2809235136</v>
       </c>
       <c r="C40" t="n">
         <v>783605.377185</v>
@@ -890,7 +890,7 @@
         <v>42775</v>
       </c>
       <c r="B41" t="n">
-        <v>947421.2890091846</v>
+        <v>949064.6568398473</v>
       </c>
       <c r="C41" t="n">
         <v>624387.4878990001</v>
@@ -901,7 +901,7 @@
         <v>42776</v>
       </c>
       <c r="B42" t="n">
-        <v>937565.523136834</v>
+        <v>939462.4535638246</v>
       </c>
       <c r="C42" t="n">
         <v>752207.2398545</v>
@@ -912,7 +912,7 @@
         <v>42777</v>
       </c>
       <c r="B43" t="n">
-        <v>1013835.693532543</v>
+        <v>1015683.420592916</v>
       </c>
       <c r="C43" t="n">
         <v>944924.65301</v>
@@ -923,7 +923,7 @@
         <v>42778</v>
       </c>
       <c r="B44" t="n">
-        <v>1118370.878350722</v>
+        <v>1119844.034742322</v>
       </c>
       <c r="C44" t="n">
         <v>1074820.900014</v>
@@ -934,7 +934,7 @@
         <v>42779</v>
       </c>
       <c r="B45" t="n">
-        <v>1204089.605303243</v>
+        <v>1205639.217204515</v>
       </c>
       <c r="C45" t="n">
         <v>794314.4320675</v>
@@ -945,7 +945,7 @@
         <v>42780</v>
       </c>
       <c r="B46" t="n">
-        <v>919281.299240188</v>
+        <v>921049.9548994583</v>
       </c>
       <c r="C46" t="n">
         <v>642613.187069</v>
@@ -956,7 +956,7 @@
         <v>42781</v>
       </c>
       <c r="B47" t="n">
-        <v>919286.9322127957</v>
+        <v>921122.6433291518</v>
       </c>
       <c r="C47" t="n">
         <v>745780.355084</v>
@@ -967,7 +967,7 @@
         <v>42782</v>
       </c>
       <c r="B48" t="n">
-        <v>951808.2547964471</v>
+        <v>953630.3704297082</v>
       </c>
       <c r="C48" t="n">
         <v>645968.2570671</v>
@@ -978,7 +978,7 @@
         <v>42783</v>
       </c>
       <c r="B49" t="n">
-        <v>941953.5604647083</v>
+        <v>944029.2244926661</v>
       </c>
       <c r="C49" t="n">
         <v>758855.71279</v>
@@ -989,7 +989,7 @@
         <v>42784</v>
       </c>
       <c r="B50" t="n">
-        <v>1018224.569426318</v>
+        <v>1020251.018918719</v>
       </c>
       <c r="C50" t="n">
         <v>1063394.844003</v>
@@ -1000,7 +1000,7 @@
         <v>42785</v>
       </c>
       <c r="B51" t="n">
-        <v>1122760.410489125</v>
+        <v>1124412.280529103</v>
       </c>
       <c r="C51" t="n">
         <v>858897.1230135</v>
@@ -1011,7 +1011,7 @@
         <v>42786</v>
       </c>
       <c r="B52" t="n">
-        <v>1208479.651005351</v>
+        <v>1210207.969647398</v>
       </c>
       <c r="C52" t="n">
         <v>759120.0599607</v>
@@ -1022,7 +1022,7 @@
         <v>42787</v>
       </c>
       <c r="B53" t="n">
-        <v>923671.7468468125</v>
+        <v>925619.1038147371</v>
       </c>
       <c r="C53" t="n">
         <v>717807.6770255</v>
@@ -1033,7 +1033,7 @@
         <v>42788</v>
       </c>
       <c r="B54" t="n">
-        <v>923677.694341725</v>
+        <v>925692.1024950328</v>
       </c>
       <c r="C54" t="n">
         <v>739388.0344027</v>
@@ -1044,7 +1044,7 @@
         <v>42789</v>
       </c>
       <c r="B55" t="n">
-        <v>956199.2630641385</v>
+        <v>958200.072375256</v>
       </c>
       <c r="C55" t="n">
         <v>675578.500156</v>
@@ -1055,7 +1055,7 @@
         <v>42790</v>
       </c>
       <c r="B56" t="n">
-        <v>946344.7613555915</v>
+        <v>948599.11642001</v>
       </c>
       <c r="C56" t="n">
         <v>816197.4989520001</v>
@@ -1066,7 +1066,7 @@
         <v>42791</v>
       </c>
       <c r="B57" t="n">
-        <v>1022615.921060196</v>
+        <v>1024821.059512066</v>
       </c>
       <c r="C57" t="n">
         <v>1026011.2228075</v>
@@ -1077,7 +1077,7 @@
         <v>42792</v>
       </c>
       <c r="B58" t="n">
-        <v>1127151.880091405</v>
+        <v>1128982.437457705</v>
       </c>
       <c r="C58" t="n">
         <v>775708.987978</v>
@@ -1088,7 +1088,7 @@
         <v>42793</v>
       </c>
       <c r="B59" t="n">
-        <v>1212871.212927306</v>
+        <v>1214778.21761155</v>
       </c>
       <c r="C59" t="n">
         <v>744956.948138</v>
@@ -1099,7 +1099,7 @@
         <v>42794</v>
       </c>
       <c r="B60" t="n">
-        <v>928063.3810162677</v>
+        <v>930189.4230167229</v>
       </c>
       <c r="C60" t="n">
         <v>949366.8290504999</v>
@@ -1110,7 +1110,7 @@
         <v>42795</v>
       </c>
       <c r="B61" t="n">
-        <v>928069.3850506053</v>
+        <v>930262.477442591</v>
       </c>
       <c r="C61" t="n">
         <v>1008521.709962</v>
@@ -1121,7 +1121,7 @@
         <v>42796</v>
       </c>
       <c r="B62" t="n">
-        <v>960590.9980196236</v>
+        <v>962770.4909452645</v>
       </c>
       <c r="C62" t="n">
         <v>836225.179072</v>
@@ -1132,7 +1132,7 @@
         <v>42797</v>
       </c>
       <c r="B63" t="n">
-        <v>950736.53093757</v>
+        <v>953169.569125791</v>
       </c>
       <c r="C63" t="n">
         <v>882639.7762739999</v>
@@ -1143,7 +1143,7 @@
         <v>42798</v>
       </c>
       <c r="B64" t="n">
-        <v>1027007.717740164</v>
+        <v>1029391.538930032</v>
       </c>
       <c r="C64" t="n">
         <v>1125736.3470592</v>
@@ -1154,7 +1154,7 @@
         <v>42799</v>
       </c>
       <c r="B65" t="n">
-        <v>1131543.69797771</v>
+        <v>1133552.937778694</v>
       </c>
       <c r="C65" t="n">
         <v>1196983.690104</v>
@@ -1165,7 +1165,7 @@
         <v>42800</v>
       </c>
       <c r="B66" t="n">
-        <v>1217263.047409258</v>
+        <v>1219348.734289732</v>
       </c>
       <c r="C66" t="n">
         <v>790143.2410905</v>
@@ -1176,7 +1176,7 @@
         <v>42801</v>
       </c>
       <c r="B67" t="n">
-        <v>932455.2284856362</v>
+        <v>934759.9524948591</v>
       </c>
       <c r="C67" t="n">
         <v>761866.729975</v>
@@ -1187,7 +1187,7 @@
         <v>42802</v>
       </c>
       <c r="B68" t="n">
-        <v>932461.2426836619</v>
+        <v>934833.0169370457</v>
       </c>
       <c r="C68" t="n">
         <v>781046.6619577</v>
@@ -1198,7 +1198,7 @@
         <v>42803</v>
       </c>
       <c r="B69" t="n">
-        <v>964982.8636065759</v>
+        <v>967341.038277765</v>
       </c>
       <c r="C69" t="n">
         <v>653901.1919827</v>
@@ -1209,7 +1209,7 @@
         <v>42804</v>
       </c>
       <c r="B70" t="n">
-        <v>955128.4027490794</v>
+        <v>957740.122591779</v>
       </c>
       <c r="C70" t="n">
         <v>773855.3068500001</v>
@@ -1220,7 +1220,7 @@
         <v>42805</v>
       </c>
       <c r="B71" t="n">
-        <v>1031399.594422886</v>
+        <v>1033962.097195644</v>
       </c>
       <c r="C71" t="n">
         <v>1001174.4340065</v>
@@ -1231,7 +1231,7 @@
         <v>42806</v>
       </c>
       <c r="B72" t="n">
-        <v>1135935.578472542</v>
+        <v>1138123.499800143</v>
       </c>
       <c r="C72" t="n">
         <v>1146006.826973</v>
@@ -1242,7 +1242,7 @@
         <v>42807</v>
       </c>
       <c r="B73" t="n">
-        <v>1221654.930887371</v>
+        <v>1223919.299250228</v>
       </c>
       <c r="C73" t="n">
         <v>754390.380036</v>
@@ -1253,7 +1253,7 @@
         <v>42808</v>
       </c>
       <c r="B74" t="n">
-        <v>936847.1142984045</v>
+        <v>939330.5197552406</v>
       </c>
       <c r="C74" t="n">
         <v>700998.0346447</v>
@@ -1264,7 +1264,7 @@
         <v>42809</v>
       </c>
       <c r="B75" t="n">
-        <v>936853.1303234837</v>
+        <v>939403.5859971511</v>
       </c>
       <c r="C75" t="n">
         <v>815621.887369</v>
@@ -1275,7 +1275,7 @@
         <v>42810</v>
       </c>
       <c r="B76" t="n">
-        <v>969374.7526762127</v>
+        <v>971911.6087462041</v>
       </c>
       <c r="C76" t="n">
         <v>699108.166824</v>
@@ -1286,7 +1286,7 @@
         <v>42811</v>
       </c>
       <c r="B77" t="n">
-        <v>959520.2929376604</v>
+        <v>962310.694162278</v>
       </c>
       <c r="C77" t="n">
         <v>812306.7742700001</v>
@@ -1297,7 +1297,7 @@
         <v>42812</v>
       </c>
       <c r="B78" t="n">
-        <v>1035791.485487129</v>
+        <v>1038532.669628535</v>
       </c>
       <c r="C78" t="n">
         <v>1038906.566154</v>
@@ -1308,7 +1308,7 @@
         <v>42813</v>
       </c>
       <c r="B79" t="n">
-        <v>1140327.470222062</v>
+        <v>1142694.07290788</v>
       </c>
       <c r="C79" t="n">
         <v>1157140.638587</v>
@@ -1319,7 +1319,7 @@
         <v>42814</v>
       </c>
       <c r="B80" t="n">
-        <v>1226046.823173174</v>
+        <v>1228489.87288605</v>
       </c>
       <c r="C80" t="n">
         <v>826428.90991</v>
@@ -1330,7 +1330,7 @@
         <v>42815</v>
       </c>
       <c r="B81" t="n">
-        <v>941239.0070038916</v>
+        <v>943901.0938043048</v>
       </c>
       <c r="C81" t="n">
         <v>746620.926177</v>
@@ -1341,7 +1341,7 @@
         <v>42816</v>
       </c>
       <c r="B82" t="n">
-        <v>941245.0233574072</v>
+        <v>943974.1603695882</v>
       </c>
       <c r="C82" t="n">
         <v>767880.804934</v>
@@ -1352,7 +1352,7 @@
         <v>42817</v>
       </c>
       <c r="B83" t="n">
-        <v>973766.6459671637</v>
+        <v>976482.1833716894</v>
       </c>
       <c r="C83" t="n">
         <v>670848.010029</v>
@@ -1363,7 +1363,7 @@
         <v>42818</v>
       </c>
       <c r="B84" t="n">
-        <v>963912.186429756</v>
+        <v>966881.2689857805</v>
       </c>
       <c r="C84" t="n">
         <v>787914.125515</v>
@@ -1374,7 +1374,7 @@
         <v>42819</v>
       </c>
       <c r="B85" t="n">
-        <v>1040183.379136637</v>
+        <v>1043103.244606992</v>
       </c>
       <c r="C85" t="n">
         <v>1038139.316887</v>
@@ -1385,7 +1385,7 @@
         <v>42820</v>
       </c>
       <c r="B86" t="n">
-        <v>1144719.363994757</v>
+        <v>1147264.648007592</v>
       </c>
       <c r="C86" t="n">
         <v>1101557.476706</v>
@@ -1396,7 +1396,7 @@
         <v>42821</v>
       </c>
       <c r="B87" t="n">
-        <v>1230438.717042272</v>
+        <v>1233060.448080649</v>
       </c>
       <c r="C87" t="n">
         <v>784103.265042</v>
@@ -1407,7 +1407,7 @@
         <v>42822</v>
       </c>
       <c r="B88" t="n">
-        <v>945630.9009484334</v>
+        <v>948471.669073154</v>
       </c>
       <c r="C88" t="n">
         <v>702943.9485770001</v>
@@ -1418,7 +1418,7 @@
         <v>42823</v>
       </c>
       <c r="B89" t="n">
-        <v>945636.9173609897</v>
+        <v>948544.7356965407</v>
       </c>
       <c r="C89" t="n">
         <v>824632.985033</v>
@@ -1429,7 +1429,7 @@
         <v>42824</v>
       </c>
       <c r="B90" t="n">
-        <v>978158.5400169502</v>
+        <v>981052.7587441094</v>
       </c>
       <c r="C90" t="n">
         <v>637624.340998</v>
@@ -1440,7 +1440,7 @@
         <v>42825</v>
       </c>
       <c r="B91" t="n">
-        <v>968304.0805157009</v>
+        <v>971451.8443937801</v>
       </c>
       <c r="C91" t="n">
         <v>878750.03788</v>
@@ -1451,7 +1451,7 @@
         <v>42826</v>
       </c>
       <c r="B92" t="n">
-        <v>1044575.273250878</v>
+        <v>1047673.820042833</v>
       </c>
       <c r="C92" t="n">
         <v>1463083.962459</v>
@@ -1462,7 +1462,7 @@
         <v>42827</v>
       </c>
       <c r="B93" t="n">
-        <v>1149111.258131143</v>
+        <v>1151835.223465221</v>
       </c>
       <c r="C93" t="n">
         <v>1138650.058898</v>
@@ -1473,7 +1473,7 @@
         <v>42828</v>
       </c>
       <c r="B94" t="n">
-        <v>1234830.611195988</v>
+        <v>1237631.023555327</v>
       </c>
       <c r="C94" t="n">
         <v>835191.622029</v>
@@ -1484,7 +1484,7 @@
         <v>42829</v>
       </c>
       <c r="B95" t="n">
-        <v>950022.7951157113</v>
+        <v>953042.244561173</v>
       </c>
       <c r="C95" t="n">
         <v>835602.6360017</v>
@@ -1495,7 +1495,7 @@
         <v>42830</v>
       </c>
       <c r="B96" t="n">
-        <v>950028.8115388809</v>
+        <v>953115.3111949997</v>
       </c>
       <c r="C96" t="n">
         <v>846631.307907</v>
@@ -1506,7 +1506,7 @@
         <v>42831</v>
       </c>
       <c r="B97" t="n">
-        <v>982550.4342031472</v>
+        <v>985623.334250738</v>
       </c>
       <c r="C97" t="n">
         <v>683059.570103</v>
@@ -1517,7 +1517,7 @@
         <v>42832</v>
       </c>
       <c r="B98" t="n">
-        <v>972695.9747083978</v>
+        <v>976022.4199068017</v>
       </c>
       <c r="C98" t="n">
         <v>765502.211925</v>
@@ -1528,7 +1528,7 @@
         <v>42833</v>
       </c>
       <c r="B99" t="n">
-        <v>1048967.167448662</v>
+        <v>1052244.395560857</v>
       </c>
       <c r="C99" t="n">
         <v>988591.469958</v>
@@ -1539,7 +1539,7 @@
         <v>42834</v>
       </c>
       <c r="B100" t="n">
-        <v>1153503.152332907</v>
+        <v>1156405.79898716</v>
       </c>
       <c r="C100" t="n">
         <v>1101713.657101</v>
@@ -1550,7 +1550,7 @@
         <v>42835</v>
       </c>
       <c r="B101" t="n">
-        <v>1239222.505400868</v>
+        <v>1242201.599080329</v>
       </c>
       <c r="C101" t="n">
         <v>739392.130988</v>
@@ -1561,7 +1561,7 @@
         <v>42836</v>
       </c>
       <c r="B102" t="n">
-        <v>954414.6893230288</v>
+        <v>957612.8200885723</v>
       </c>
       <c r="C102" t="n">
         <v>741331.430196</v>
@@ -1572,7 +1572,7 @@
         <v>42837</v>
       </c>
       <c r="B103" t="n">
-        <v>954420.7057481064</v>
+        <v>957685.886724275</v>
       </c>
       <c r="C103" t="n">
         <v>791762.312883</v>
@@ -1583,7 +1583,7 @@
         <v>42838</v>
       </c>
       <c r="B104" t="n">
-        <v>986942.3284138656</v>
+        <v>990193.9097814811</v>
       </c>
       <c r="C104" t="n">
         <v>737029.5651830001</v>
@@ -1594,7 +1594,7 @@
         <v>42839</v>
       </c>
       <c r="B105" t="n">
-        <v>977087.8689202847</v>
+        <v>980592.9954386934</v>
       </c>
       <c r="C105" t="n">
         <v>740889.4868289999</v>
@@ -1605,7 +1605,7 @@
         <v>42840</v>
       </c>
       <c r="B106" t="n">
-        <v>1053359.061661463</v>
+        <v>1056814.971093648</v>
       </c>
       <c r="C106" t="n">
         <v>898610.217928</v>
@@ -1616,7 +1616,7 @@
         <v>42841</v>
       </c>
       <c r="B107" t="n">
-        <v>1157895.046546424</v>
+        <v>1160976.374520654</v>
       </c>
       <c r="C107" t="n">
         <v>985493.795113</v>
@@ -1627,7 +1627,7 @@
         <v>42842</v>
       </c>
       <c r="B108" t="n">
-        <v>1243614.399614945</v>
+        <v>1246772.174614373</v>
       </c>
       <c r="C108" t="n">
         <v>775916.9059055001</v>
@@ -1638,7 +1638,7 @@
         <v>42843</v>
       </c>
       <c r="B109" t="n">
-        <v>958806.583537544</v>
+        <v>962183.3956230475</v>
       </c>
       <c r="C109" t="n">
         <v>717196.315762</v>
@@ -1649,7 +1649,7 @@
         <v>42844</v>
       </c>
       <c r="B110" t="n">
-        <v>958812.5999629645</v>
+        <v>962256.4622590871</v>
       </c>
       <c r="C110" t="n">
         <v>735733.2142477001</v>
@@ -1660,7 +1660,7 @@
         <v>42845</v>
       </c>
       <c r="B111" t="n">
-        <v>991334.2226289922</v>
+        <v>994764.4853165571</v>
       </c>
       <c r="C111" t="n">
         <v>675804.0219027</v>
@@ -1671,7 +1671,7 @@
         <v>42846</v>
       </c>
       <c r="B112" t="n">
-        <v>981479.7631356212</v>
+        <v>985163.5709739758</v>
       </c>
       <c r="C112" t="n">
         <v>795795.893872</v>
@@ -1682,7 +1682,7 @@
         <v>42847</v>
       </c>
       <c r="B113" t="n">
-        <v>1057750.955876964</v>
+        <v>1061385.546629092</v>
       </c>
       <c r="C113" t="n">
         <v>974952.817869</v>
@@ -1693,7 +1693,7 @@
         <v>42848</v>
       </c>
       <c r="B114" t="n">
-        <v>1162286.940762054</v>
+        <v>1165546.950056224</v>
       </c>
       <c r="C114" t="n">
         <v>1140070.2748035</v>
@@ -1704,7 +1704,7 @@
         <v>42849</v>
       </c>
       <c r="B115" t="n">
-        <v>1248006.293830675</v>
+        <v>1251342.750150042</v>
       </c>
       <c r="C115" t="n">
         <v>755072.530945</v>
@@ -1715,7 +1715,7 @@
         <v>42850</v>
       </c>
       <c r="B116" t="n">
-        <v>963198.4777533531</v>
+        <v>966753.971158794</v>
       </c>
       <c r="C116" t="n">
         <v>718996.080637</v>
@@ -1726,7 +1726,7 @@
         <v>42851</v>
       </c>
       <c r="B117" t="n">
-        <v>963204.4941788352</v>
+        <v>966827.0377948942</v>
       </c>
       <c r="C117" t="n">
         <v>781159.2829995001</v>
@@ -1737,7 +1737,7 @@
         <v>42852</v>
       </c>
       <c r="B118" t="n">
-        <v>995726.1168449111</v>
+        <v>999335.0608524116</v>
       </c>
       <c r="C118" t="n">
         <v>624910.0260955</v>
@@ -1748,7 +1748,7 @@
         <v>42853</v>
       </c>
       <c r="B119" t="n">
-        <v>985871.6573515779</v>
+        <v>989734.1465098674</v>
       </c>
       <c r="C119" t="n">
         <v>797636.6251025</v>
@@ -1759,7 +1759,7 @@
         <v>42854</v>
       </c>
       <c r="B120" t="n">
-        <v>1062142.85009295</v>
+        <v>1065956.122165012</v>
       </c>
       <c r="C120" t="n">
         <v>1068279.815941</v>
@@ -1770,7 +1770,7 @@
         <v>42855</v>
       </c>
       <c r="B121" t="n">
-        <v>1166678.834978063</v>
+        <v>1170117.525592168</v>
       </c>
       <c r="C121" t="n">
         <v>1041249.2479705</v>
@@ -1781,7 +1781,7 @@
         <v>42856</v>
       </c>
       <c r="B122" t="n">
-        <v>1252398.188046703</v>
+        <v>1255913.325686003</v>
       </c>
       <c r="C122" t="n">
         <v>1306699.366897</v>
@@ -1792,7 +1792,7 @@
         <v>42857</v>
       </c>
       <c r="B123" t="n">
-        <v>967590.3719693947</v>
+        <v>971324.5466947689</v>
       </c>
       <c r="C123" t="n">
         <v>907324.094113</v>
@@ -1803,7 +1803,7 @@
         <v>42858</v>
       </c>
       <c r="B124" t="n">
-        <v>967596.3883948879</v>
+        <v>971397.6133308801</v>
       </c>
       <c r="C124" t="n">
         <v>924247.257204</v>
@@ -1814,7 +1814,7 @@
         <v>42859</v>
       </c>
       <c r="B125" t="n">
-        <v>1000118.011060972</v>
+        <v>1003905.636388406</v>
       </c>
       <c r="C125" t="n">
         <v>716654.608983</v>
@@ -1825,7 +1825,7 @@
         <v>42860</v>
       </c>
       <c r="B126" t="n">
-        <v>990263.5515676461</v>
+        <v>994304.7220458684</v>
       </c>
       <c r="C126" t="n">
         <v>780798.407016</v>
@@ -1836,7 +1836,7 @@
         <v>42861</v>
       </c>
       <c r="B127" t="n">
-        <v>1066534.744309024</v>
+        <v>1070526.697701019</v>
       </c>
       <c r="C127" t="n">
         <v>1039417.861868</v>
@@ -1847,7 +1847,7 @@
         <v>42862</v>
       </c>
       <c r="B128" t="n">
-        <v>1171070.729194141</v>
+        <v>1174688.101128178</v>
       </c>
       <c r="C128" t="n">
         <v>1227380.607924</v>
@@ -1858,7 +1858,7 @@
         <v>42863</v>
       </c>
       <c r="B129" t="n">
-        <v>1256790.082262784</v>
+        <v>1260483.901222017</v>
       </c>
       <c r="C129" t="n">
         <v>776307.495015</v>
@@ -1869,7 +1869,7 @@
         <v>42864</v>
       </c>
       <c r="B130" t="n">
-        <v>971982.2661854782</v>
+        <v>975895.122230785</v>
       </c>
       <c r="C130" t="n">
         <v>715811.198881</v>
@@ -1880,7 +1880,7 @@
         <v>42865</v>
       </c>
       <c r="B131" t="n">
-        <v>971988.2826109733</v>
+        <v>975968.1888668981</v>
       </c>
       <c r="C131" t="n">
         <v>766101.907094</v>
@@ -1891,7 +1891,7 @@
         <v>42866</v>
       </c>
       <c r="B132" t="n">
-        <v>1004509.905277059</v>
+        <v>1008476.211924425</v>
       </c>
       <c r="C132" t="n">
         <v>648650.413039</v>
@@ -1902,7 +1902,7 @@
         <v>42867</v>
       </c>
       <c r="B133" t="n">
-        <v>994655.4457837343</v>
+        <v>998875.2975818891</v>
       </c>
       <c r="C133" t="n">
         <v>764812.415784</v>
@@ -1913,7 +1913,7 @@
         <v>42868</v>
       </c>
       <c r="B134" t="n">
-        <v>1070926.638525113</v>
+        <v>1075097.27323704</v>
       </c>
       <c r="C134" t="n">
         <v>1116976.891153</v>
@@ -1924,7 +1924,7 @@
         <v>42869</v>
       </c>
       <c r="B135" t="n">
-        <v>1175462.623410231</v>
+        <v>1179258.6766642</v>
       </c>
       <c r="C135" t="n">
         <v>884199.9138385</v>
@@ -1935,7 +1935,7 @@
         <v>42870</v>
       </c>
       <c r="B136" t="n">
-        <v>1261181.976478874</v>
+        <v>1265054.47675804</v>
       </c>
       <c r="C136" t="n">
         <v>823035.572122</v>
@@ -1946,7 +1946,7 @@
         <v>42871</v>
       </c>
       <c r="B137" t="n">
-        <v>976374.1604015691</v>
+        <v>980465.6977668083</v>
       </c>
       <c r="C137" t="n">
         <v>807803.8950783</v>
@@ -1957,7 +1957,7 @@
         <v>42872</v>
       </c>
       <c r="B138" t="n">
-        <v>976380.1768270647</v>
+        <v>980538.7644029218</v>
       </c>
       <c r="C138" t="n">
         <v>841407.607944</v>
@@ -1968,7 +1968,7 @@
         <v>42873</v>
       </c>
       <c r="B139" t="n">
-        <v>1008901.799493151</v>
+        <v>1013046.78746045</v>
       </c>
       <c r="C139" t="n">
         <v>628487.9899620001</v>
@@ -1979,7 +1979,7 @@
         <v>42874</v>
       </c>
       <c r="B140" t="n">
-        <v>999047.3399998262</v>
+        <v>1003445.873117913</v>
       </c>
       <c r="C140" t="n">
         <v>773775.4378677</v>
@@ -1990,7 +1990,7 @@
         <v>42875</v>
       </c>
       <c r="B141" t="n">
-        <v>1075318.532741205</v>
+        <v>1079667.848773065</v>
       </c>
       <c r="C141" t="n">
         <v>1035667.381833</v>
@@ -2001,7 +2001,7 @@
         <v>42876</v>
       </c>
       <c r="B142" t="n">
-        <v>1179854.517626323</v>
+        <v>1183829.252200225</v>
       </c>
       <c r="C142" t="n">
         <v>1201938.886229</v>
@@ -2012,7 +2012,7 @@
         <v>42877</v>
       </c>
       <c r="B143" t="n">
-        <v>1265573.870694966</v>
+        <v>1269625.052294065</v>
       </c>
       <c r="C143" t="n">
         <v>778935.156126</v>
@@ -2023,7 +2023,7 @@
         <v>42878</v>
       </c>
       <c r="B144" t="n">
-        <v>980766.0546176614</v>
+        <v>985036.2733028331</v>
       </c>
       <c r="C144" t="n">
         <v>723151.767982</v>
@@ -2034,7 +2034,7 @@
         <v>42879</v>
       </c>
       <c r="B145" t="n">
-        <v>980772.0710431571</v>
+        <v>985109.3399389465</v>
       </c>
       <c r="C145" t="n">
         <v>746303.6271255</v>
@@ -2045,7 +2045,7 @@
         <v>42880</v>
       </c>
       <c r="B146" t="n">
-        <v>1013293.693709243</v>
+        <v>1017617.362996474</v>
       </c>
       <c r="C146" t="n">
         <v>620108.24391</v>
@@ -2056,7 +2056,7 @@
         <v>42881</v>
       </c>
       <c r="B147" t="n">
-        <v>1003439.234215919</v>
+        <v>1008016.448653938</v>
       </c>
       <c r="C147" t="n">
         <v>984511.1521135001</v>
@@ -2067,7 +2067,7 @@
         <v>42882</v>
       </c>
       <c r="B148" t="n">
-        <v>1079710.426957298</v>
+        <v>1084238.42430909</v>
       </c>
       <c r="C148" t="n">
         <v>932219.893144</v>
@@ -2078,7 +2078,7 @@
         <v>42883</v>
       </c>
       <c r="B149" t="n">
-        <v>1184246.411842415</v>
+        <v>1188399.82773625</v>
       </c>
       <c r="C149" t="n">
         <v>1061771.636907</v>
@@ -2089,7 +2089,7 @@
         <v>42884</v>
       </c>
       <c r="B150" t="n">
-        <v>1269965.764911059</v>
+        <v>1274195.62783009</v>
       </c>
       <c r="C150" t="n">
         <v>776813.137038</v>
@@ -2100,7 +2100,7 @@
         <v>42885</v>
       </c>
       <c r="B151" t="n">
-        <v>985157.9488337539</v>
+        <v>989606.8488388581</v>
       </c>
       <c r="C151" t="n">
         <v>742471.2769905</v>
@@ -2111,7 +2111,7 @@
         <v>42886</v>
       </c>
       <c r="B152" t="n">
-        <v>985163.9652592497</v>
+        <v>989679.9154749715</v>
       </c>
       <c r="C152" t="n">
         <v>858062.149411</v>
@@ -2122,7 +2122,7 @@
         <v>42887</v>
       </c>
       <c r="B153" t="n">
-        <v>1017685.587925336</v>
+        <v>1022187.938532499</v>
       </c>
       <c r="C153" t="n">
         <v>766859.1728450001</v>
@@ -2133,7 +2133,7 @@
         <v>42888</v>
       </c>
       <c r="B154" t="n">
-        <v>1007831.128432011</v>
+        <v>1012587.024189963</v>
       </c>
       <c r="C154" t="n">
         <v>918421.319125</v>
@@ -2144,7 +2144,7 @@
         <v>42889</v>
       </c>
       <c r="B155" t="n">
-        <v>1084102.32117339</v>
+        <v>1088808.999845115</v>
       </c>
       <c r="C155" t="n">
         <v>1176138.109152</v>
@@ -2155,7 +2155,7 @@
         <v>42890</v>
       </c>
       <c r="B156" t="n">
-        <v>1188638.306058508</v>
+        <v>1192970.403272275</v>
       </c>
       <c r="C156" t="n">
         <v>1376511.520495</v>
@@ -2166,7 +2166,7 @@
         <v>42891</v>
       </c>
       <c r="B157" t="n">
-        <v>1274357.659127151</v>
+        <v>1278766.203366115</v>
       </c>
       <c r="C157" t="n">
         <v>912693.8511</v>
@@ -2177,7 +2177,7 @@
         <v>42892</v>
       </c>
       <c r="B158" t="n">
-        <v>989549.8430498465</v>
+        <v>994177.4243748831</v>
       </c>
       <c r="C158" t="n">
         <v>805546.6479559999</v>
@@ -2188,7 +2188,7 @@
         <v>42893</v>
       </c>
       <c r="B159" t="n">
-        <v>989555.8594753423</v>
+        <v>994250.4910109965</v>
       </c>
       <c r="C159" t="n">
         <v>842979.8370823</v>
@@ -2199,7 +2199,7 @@
         <v>42894</v>
       </c>
       <c r="B160" t="n">
-        <v>1022077.482141429</v>
+        <v>1026758.514068524</v>
       </c>
       <c r="C160" t="n">
         <v>667099.8010250001</v>
@@ -2210,7 +2210,7 @@
         <v>42895</v>
       </c>
       <c r="B161" t="n">
-        <v>1012223.022648104</v>
+        <v>1017157.599725988</v>
       </c>
       <c r="C161" t="n">
         <v>795116.1360699</v>
@@ -2221,7 +2221,7 @@
         <v>42896</v>
       </c>
       <c r="B162" t="n">
-        <v>1088494.215389483</v>
+        <v>1093379.57538114</v>
       </c>
       <c r="C162" t="n">
         <v>993732.684049</v>
@@ -2232,7 +2232,7 @@
         <v>42897</v>
       </c>
       <c r="B163" t="n">
-        <v>1193030.2002746</v>
+        <v>1197540.9788083</v>
       </c>
       <c r="C163" t="n">
         <v>1213673.946877</v>
@@ -2243,7 +2243,7 @@
         <v>42898</v>
       </c>
       <c r="B164" t="n">
-        <v>1278749.553343244</v>
+        <v>1283336.77890214</v>
       </c>
       <c r="C164" t="n">
         <v>768349.7589516999</v>
@@ -2254,7 +2254,7 @@
         <v>42899</v>
       </c>
       <c r="B165" t="n">
-        <v>993941.7372659391</v>
+        <v>998747.9999109081</v>
       </c>
       <c r="C165" t="n">
         <v>729412.959849</v>
@@ -2265,7 +2265,7 @@
         <v>42900</v>
       </c>
       <c r="B166" t="n">
-        <v>993947.753691435</v>
+        <v>998821.0665470215</v>
       </c>
       <c r="C166" t="n">
         <v>785885.9088963</v>
@@ -2276,7 +2276,7 @@
         <v>42901</v>
       </c>
       <c r="B167" t="n">
-        <v>1026469.376357521</v>
+        <v>1031329.089604549</v>
       </c>
       <c r="C167" t="n">
         <v>660338.346974</v>
@@ -2287,7 +2287,7 @@
         <v>42902</v>
       </c>
       <c r="B168" t="n">
-        <v>1016614.916864196</v>
+        <v>1021728.175262013</v>
       </c>
       <c r="C168" t="n">
         <v>834786.4275550001</v>
@@ -2298,7 +2298,7 @@
         <v>42903</v>
       </c>
       <c r="B169" t="n">
-        <v>1092886.109605575</v>
+        <v>1097950.150917165</v>
       </c>
       <c r="C169" t="n">
         <v>1096133.5508865</v>
@@ -2309,7 +2309,7 @@
         <v>42904</v>
       </c>
       <c r="B170" t="n">
-        <v>1197422.094490693</v>
+        <v>1202111.554344325</v>
       </c>
       <c r="C170" t="n">
         <v>965144.121179</v>
@@ -2320,7 +2320,7 @@
         <v>42905</v>
       </c>
       <c r="B171" t="n">
-        <v>1283141.447559336</v>
+        <v>1287907.354438165</v>
       </c>
       <c r="C171" t="n">
         <v>791146.393731</v>
@@ -2331,7 +2331,7 @@
         <v>42906</v>
       </c>
       <c r="B172" t="n">
-        <v>998333.6314820318</v>
+        <v>1003318.575446933</v>
       </c>
       <c r="C172" t="n">
         <v>787326.7170395</v>
@@ -2342,7 +2342,7 @@
         <v>42907</v>
       </c>
       <c r="B173" t="n">
-        <v>998339.6479075276</v>
+        <v>1003391.642083046</v>
       </c>
       <c r="C173" t="n">
         <v>766159.0112892</v>
@@ -2353,7 +2353,7 @@
         <v>42908</v>
       </c>
       <c r="B174" t="n">
-        <v>1030861.270573614</v>
+        <v>1035899.665140574</v>
       </c>
       <c r="C174" t="n">
         <v>609868.8309586</v>
@@ -2364,7 +2364,7 @@
         <v>42909</v>
       </c>
       <c r="B175" t="n">
-        <v>1021006.811080289</v>
+        <v>1026298.750798038</v>
       </c>
       <c r="C175" t="n">
         <v>761049.7450639</v>
@@ -2375,7 +2375,7 @@
         <v>42910</v>
       </c>
       <c r="B176" t="n">
-        <v>1097278.003821668</v>
+        <v>1102520.72645319</v>
       </c>
       <c r="C176" t="n">
         <v>963268.2271350001</v>
@@ -2386,7 +2386,7 @@
         <v>42911</v>
       </c>
       <c r="B177" t="n">
-        <v>1201813.988706785</v>
+        <v>1206682.12988035</v>
       </c>
       <c r="C177" t="n">
         <v>1092610.858614</v>
@@ -2397,7 +2397,7 @@
         <v>42912</v>
       </c>
       <c r="B178" t="n">
-        <v>1287533.341775429</v>
+        <v>1292477.929974189</v>
       </c>
       <c r="C178" t="n">
         <v>755367.8450665</v>
@@ -2408,7 +2408,7 @@
         <v>42913</v>
       </c>
       <c r="B179" t="n">
-        <v>1002725.525698124</v>
+        <v>1007889.150982958</v>
       </c>
       <c r="C179" t="n">
         <v>682218.468913</v>
@@ -2419,7 +2419,7 @@
         <v>42914</v>
       </c>
       <c r="B180" t="n">
-        <v>1002731.54212362</v>
+        <v>1007962.217619071</v>
       </c>
       <c r="C180" t="n">
         <v>731896.9850104999</v>
@@ -2430,7 +2430,7 @@
         <v>42915</v>
       </c>
       <c r="B181" t="n">
-        <v>1035253.164789707</v>
+        <v>1040470.240676599</v>
       </c>
       <c r="C181" t="n">
         <v>630811.802872</v>
@@ -2441,7 +2441,7 @@
         <v>42916</v>
       </c>
       <c r="B182" t="n">
-        <v>1025398.705296382</v>
+        <v>1030869.326334063</v>
       </c>
       <c r="C182" t="n">
         <v>802273.1392327</v>
@@ -2452,7 +2452,7 @@
         <v>42917</v>
       </c>
       <c r="B183" t="n">
-        <v>1101669.89803776</v>
+        <v>1107091.301989215</v>
       </c>
       <c r="C183" t="n">
         <v>1207529.921868</v>
@@ -2463,7 +2463,7 @@
         <v>42918</v>
       </c>
       <c r="B184" t="n">
-        <v>1206205.882922878</v>
+        <v>1211252.705416375</v>
       </c>
       <c r="C184" t="n">
         <v>1296379.2175535</v>
@@ -2474,7 +2474,7 @@
         <v>42919</v>
       </c>
       <c r="B185" t="n">
-        <v>1291925.235991522</v>
+        <v>1297048.505510214</v>
       </c>
       <c r="C185" t="n">
         <v>925143.408816</v>
@@ -2485,7 +2485,7 @@
         <v>42920</v>
       </c>
       <c r="B186" t="n">
-        <v>1007117.419914217</v>
+        <v>1012459.726518983</v>
       </c>
       <c r="C186" t="n">
         <v>832359.2860137</v>
@@ -2496,7 +2496,7 @@
         <v>42921</v>
       </c>
       <c r="B187" t="n">
-        <v>1007123.436339713</v>
+        <v>1012532.793155096</v>
       </c>
       <c r="C187" t="n">
         <v>844301.613116</v>
@@ -2507,7 +2507,7 @@
         <v>42922</v>
       </c>
       <c r="B188" t="n">
-        <v>1039645.059005799</v>
+        <v>1045040.816212624</v>
       </c>
       <c r="C188" t="n">
         <v>700272.0099567</v>
@@ -2518,7 +2518,7 @@
         <v>42923</v>
       </c>
       <c r="B189" t="n">
-        <v>1029790.599512474</v>
+        <v>1035439.901870088</v>
       </c>
       <c r="C189" t="n">
         <v>805792.302193</v>
@@ -2529,7 +2529,7 @@
         <v>42924</v>
       </c>
       <c r="B190" t="n">
-        <v>1106061.792253853</v>
+        <v>1111661.87752524</v>
       </c>
       <c r="C190" t="n">
         <v>998347.1930085</v>
@@ -2540,7 +2540,7 @@
         <v>42925</v>
       </c>
       <c r="B191" t="n">
-        <v>1210597.777138971</v>
+        <v>1215823.2809524</v>
       </c>
       <c r="C191" t="n">
         <v>1100833.322376</v>
@@ -2551,7 +2551,7 @@
         <v>42926</v>
       </c>
       <c r="B192" t="n">
-        <v>1296317.130207614</v>
+        <v>1301619.081046239</v>
       </c>
       <c r="C192" t="n">
         <v>804158.8610365</v>
@@ -2562,7 +2562,7 @@
         <v>42927</v>
       </c>
       <c r="B193" t="n">
-        <v>1011509.31413031</v>
+        <v>1017030.302055008</v>
       </c>
       <c r="C193" t="n">
         <v>730534.767701</v>
@@ -2573,7 +2573,7 @@
         <v>42928</v>
       </c>
       <c r="B194" t="n">
-        <v>1011515.330555806</v>
+        <v>1017103.368691121</v>
       </c>
       <c r="C194" t="n">
         <v>748799.9959087</v>
@@ -2584,7 +2584,7 @@
         <v>42929</v>
       </c>
       <c r="B195" t="n">
-        <v>1044036.953221892</v>
+        <v>1049611.391748649</v>
       </c>
       <c r="C195" t="n">
         <v>629651.3629294999</v>
@@ -2595,7 +2595,7 @@
         <v>42930</v>
       </c>
       <c r="B196" t="n">
-        <v>1034182.493728567</v>
+        <v>1040010.477406113</v>
       </c>
       <c r="C196" t="n">
         <v>765489.6173932999</v>
@@ -2606,7 +2606,7 @@
         <v>42931</v>
       </c>
       <c r="B197" t="n">
-        <v>1110453.686469945</v>
+        <v>1116232.453061265</v>
       </c>
       <c r="C197" t="n">
         <v>969077.125075</v>
@@ -2617,7 +2617,7 @@
         <v>42932</v>
       </c>
       <c r="B198" t="n">
-        <v>1214989.671355063</v>
+        <v>1220393.856488425</v>
       </c>
       <c r="C198" t="n">
         <v>1100803.699023</v>
@@ -2628,7 +2628,7 @@
         <v>42933</v>
       </c>
       <c r="B199" t="n">
-        <v>1300709.024423707</v>
+        <v>1306189.656582264</v>
       </c>
       <c r="C199" t="n">
         <v>818325.522149</v>
@@ -2639,7 +2639,7 @@
         <v>42934</v>
       </c>
       <c r="B200" t="n">
-        <v>1015901.208346402</v>
+        <v>1021600.877591033</v>
       </c>
       <c r="C200" t="n">
         <v>730133.70894</v>
@@ -2650,7 +2650,7 @@
         <v>42935</v>
       </c>
       <c r="B201" t="n">
-        <v>1015907.224771898</v>
+        <v>1021673.944227146</v>
       </c>
       <c r="C201" t="n">
         <v>767978.7780779999</v>
@@ -2661,7 +2661,7 @@
         <v>42936</v>
       </c>
       <c r="B202" t="n">
-        <v>1048428.847437985</v>
+        <v>1054181.967284674</v>
       </c>
       <c r="C202" t="n">
         <v>688288.067857</v>
@@ -2672,7 +2672,7 @@
         <v>42937</v>
       </c>
       <c r="B203" t="n">
-        <v>1038574.38794466</v>
+        <v>1044581.052942138</v>
       </c>
       <c r="C203" t="n">
         <v>782418.2992188</v>
@@ -2683,7 +2683,7 @@
         <v>42938</v>
       </c>
       <c r="B204" t="n">
-        <v>1114845.580686038</v>
+        <v>1120803.02859729</v>
       </c>
       <c r="C204" t="n">
         <v>932902.046681</v>
@@ -2694,7 +2694,7 @@
         <v>42939</v>
       </c>
       <c r="B205" t="n">
-        <v>1219381.565571156</v>
+        <v>1224964.43202445</v>
       </c>
       <c r="C205" t="n">
         <v>1024288.741245</v>
@@ -2705,7 +2705,7 @@
         <v>42940</v>
       </c>
       <c r="B206" t="n">
-        <v>1305100.918639799</v>
+        <v>1310760.232118289</v>
       </c>
       <c r="C206" t="n">
         <v>816564.327096</v>
@@ -2716,7 +2716,7 @@
         <v>42941</v>
       </c>
       <c r="B207" t="n">
-        <v>1020293.102562495</v>
+        <v>1026171.453127058</v>
       </c>
       <c r="C207" t="n">
         <v>713581.632609</v>
@@ -2727,7 +2727,7 @@
         <v>42942</v>
       </c>
       <c r="B208" t="n">
-        <v>1020299.118987991</v>
+        <v>1026244.519763171</v>
       </c>
       <c r="C208" t="n">
         <v>740653.044167</v>
@@ -2738,7 +2738,7 @@
         <v>42943</v>
       </c>
       <c r="B209" t="n">
-        <v>1052820.741654077</v>
+        <v>1058752.542820699</v>
       </c>
       <c r="C209" t="n">
         <v>659849.8270588</v>
@@ -2749,7 +2749,7 @@
         <v>42944</v>
       </c>
       <c r="B210" t="n">
-        <v>1042966.282160752</v>
+        <v>1049151.628478163</v>
       </c>
       <c r="C210" t="n">
         <v>835099.6822034999</v>
@@ -2760,7 +2760,7 @@
         <v>42945</v>
       </c>
       <c r="B211" t="n">
-        <v>1119237.47490213</v>
+        <v>1125373.604133315</v>
       </c>
       <c r="C211" t="n">
         <v>1032310.865737</v>
@@ -2771,7 +2771,7 @@
         <v>42946</v>
       </c>
       <c r="B212" t="n">
-        <v>1223773.459787248</v>
+        <v>1229535.007560475</v>
       </c>
       <c r="C212" t="n">
         <v>1123752.4779517</v>
@@ -2782,7 +2782,7 @@
         <v>42947</v>
       </c>
       <c r="B213" t="n">
-        <v>1309492.812855892</v>
+        <v>1315330.807654314</v>
       </c>
       <c r="C213" t="n">
         <v>885856.8408705</v>
@@ -2793,7 +2793,7 @@
         <v>42948</v>
       </c>
       <c r="B214" t="n">
-        <v>1024684.996778588</v>
+        <v>1030742.028663083</v>
       </c>
       <c r="C214" t="n">
         <v>988527.763204</v>
@@ -2804,7 +2804,7 @@
         <v>42949</v>
       </c>
       <c r="B215" t="n">
-        <v>1024691.013204084</v>
+        <v>1030815.095299196</v>
       </c>
       <c r="C215" t="n">
         <v>964712.016051</v>
@@ -2815,7 +2815,7 @@
         <v>42950</v>
       </c>
       <c r="B216" t="n">
-        <v>1057212.63587017</v>
+        <v>1063323.118356724</v>
       </c>
       <c r="C216" t="n">
         <v>728068.4851319999</v>
@@ -2826,7 +2826,7 @@
         <v>42951</v>
       </c>
       <c r="B217" t="n">
-        <v>1047358.176376845</v>
+        <v>1053722.204014188</v>
       </c>
       <c r="C217" t="n">
         <v>827775.686128</v>
@@ -2837,7 +2837,7 @@
         <v>42952</v>
       </c>
       <c r="B218" t="n">
-        <v>1123629.369118223</v>
+        <v>1129944.17966934</v>
       </c>
       <c r="C218" t="n">
         <v>965693.650492</v>
@@ -2848,7 +2848,7 @@
         <v>42953</v>
       </c>
       <c r="B219" t="n">
-        <v>1228165.354003341</v>
+        <v>1234105.5830965</v>
       </c>
       <c r="C219" t="n">
         <v>1049559.164277</v>
@@ -2859,7 +2859,7 @@
         <v>42954</v>
       </c>
       <c r="B220" t="n">
-        <v>1313884.707071984</v>
+        <v>1319901.383190339</v>
       </c>
       <c r="C220" t="n">
         <v>797464.963817</v>
@@ -2870,7 +2870,7 @@
         <v>42955</v>
       </c>
       <c r="B221" t="n">
-        <v>1029076.89099468</v>
+        <v>1035312.604199108</v>
       </c>
       <c r="C221" t="n">
         <v>717766.3491055</v>
@@ -2881,7 +2881,7 @@
         <v>42956</v>
       </c>
       <c r="B222" t="n">
-        <v>1029082.907420176</v>
+        <v>1035385.670835221</v>
       </c>
       <c r="C222" t="n">
         <v>734139.67401</v>
@@ -2892,7 +2892,7 @@
         <v>42957</v>
       </c>
       <c r="B223" t="n">
-        <v>1061604.530086262</v>
+        <v>1067893.693892749</v>
       </c>
       <c r="C223" t="n">
         <v>651386.9119697</v>
@@ -2903,7 +2903,7 @@
         <v>42958</v>
       </c>
       <c r="B224" t="n">
-        <v>1051750.070592938</v>
+        <v>1058292.779550213</v>
       </c>
       <c r="C224" t="n">
         <v>826373.722022</v>
@@ -2914,7 +2914,7 @@
         <v>42959</v>
       </c>
       <c r="B225" t="n">
-        <v>1128021.263334316</v>
+        <v>1134514.755205365</v>
       </c>
       <c r="C225" t="n">
         <v>792630.5350785</v>
@@ -2925,7 +2925,7 @@
         <v>42960</v>
       </c>
       <c r="B226" t="n">
-        <v>1232557.248219433</v>
+        <v>1238676.158632525</v>
       </c>
       <c r="C226" t="n">
         <v>865639.677471</v>
@@ -2936,7 +2936,7 @@
         <v>42961</v>
       </c>
       <c r="B227" t="n">
-        <v>1318276.601288077</v>
+        <v>1324471.958726364</v>
       </c>
       <c r="C227" t="n">
         <v>760922.4060808</v>
@@ -2947,7 +2947,7 @@
         <v>42962</v>
       </c>
       <c r="B228" t="n">
-        <v>1033468.785210773</v>
+        <v>1039883.179735133</v>
       </c>
       <c r="C228" t="n">
         <v>762661.935939</v>

</xml_diff>

<commit_message>
modified:   README.md modified:   models/prophet_model.joblib modified:   models/sarima_model.joblib modified:   outputs/SARIMA_sales_forecast.xlsx modified:   outputs/prophet_sales_forecast.xlsx
</commit_message>
<xml_diff>
--- a/outputs/SARIMA_sales_forecast.xlsx
+++ b/outputs/SARIMA_sales_forecast.xlsx
@@ -461,7 +461,7 @@
         <v>42736</v>
       </c>
       <c r="B2" t="n">
-        <v>1153682.926250385</v>
+        <v>1153669.444164764</v>
       </c>
       <c r="C2" t="n">
         <v>12082.500997</v>
@@ -472,7 +472,7 @@
         <v>42737</v>
       </c>
       <c r="B3" t="n">
-        <v>1246758.041321444</v>
+        <v>1246804.930994407</v>
       </c>
       <c r="C3" t="n">
         <v>1402306.370834</v>
@@ -483,7 +483,7 @@
         <v>42738</v>
       </c>
       <c r="B4" t="n">
-        <v>948943.3902764432</v>
+        <v>948951.173119908</v>
       </c>
       <c r="C4" t="n">
         <v>1104377.0798245</v>
@@ -494,7 +494,7 @@
         <v>42739</v>
       </c>
       <c r="B5" t="n">
-        <v>932933.6798767837</v>
+        <v>932905.2588968549</v>
       </c>
       <c r="C5" t="n">
         <v>990093.4637420001</v>
@@ -505,7 +505,7 @@
         <v>42740</v>
       </c>
       <c r="B6" t="n">
-        <v>957450.9911664735</v>
+        <v>957406.623702239</v>
       </c>
       <c r="C6" t="n">
         <v>777620.9540695</v>
@@ -516,7 +516,7 @@
         <v>42741</v>
       </c>
       <c r="B7" t="n">
-        <v>941670.5007358722</v>
+        <v>941623.5339444641</v>
       </c>
       <c r="C7" t="n">
         <v>839600.237989</v>
@@ -527,7 +527,7 @@
         <v>42742</v>
       </c>
       <c r="B8" t="n">
-        <v>1012215.840446734</v>
+        <v>1012133.780597739</v>
       </c>
       <c r="C8" t="n">
         <v>1103806.298949</v>
@@ -538,7 +538,7 @@
         <v>42743</v>
       </c>
       <c r="B9" t="n">
-        <v>1112097.080020959</v>
+        <v>1111976.849638395</v>
       </c>
       <c r="C9" t="n">
         <v>1192543.750978</v>
@@ -549,7 +549,7 @@
         <v>42744</v>
       </c>
       <c r="B10" t="n">
-        <v>1194660.925585052</v>
+        <v>1194524.076488608</v>
       </c>
       <c r="C10" t="n">
         <v>793724.8969065</v>
@@ -560,7 +560,7 @@
         <v>42745</v>
       </c>
       <c r="B11" t="n">
-        <v>907489.4978352296</v>
+        <v>907331.2223863428</v>
       </c>
       <c r="C11" t="n">
         <v>742635.5692609</v>
@@ -571,7 +571,7 @@
         <v>42746</v>
       </c>
       <c r="B12" t="n">
-        <v>905531.6284224122</v>
+        <v>905355.0258405533</v>
       </c>
       <c r="C12" t="n">
         <v>770742.690065</v>
@@ -582,7 +582,7 @@
         <v>42747</v>
       </c>
       <c r="B13" t="n">
-        <v>936462.0827977078</v>
+        <v>936264.3934685236</v>
       </c>
       <c r="C13" t="n">
         <v>629635.794004</v>
@@ -593,7 +593,7 @@
         <v>42748</v>
       </c>
       <c r="B14" t="n">
-        <v>925626.0283044118</v>
+        <v>925431.7162882519</v>
       </c>
       <c r="C14" t="n">
         <v>768898.9443881999</v>
@@ -604,7 +604,7 @@
         <v>42749</v>
       </c>
       <c r="B15" t="n">
-        <v>1000879.506205412</v>
+        <v>1000661.468290279</v>
       </c>
       <c r="C15" t="n">
         <v>1021050.536226</v>
@@ -615,7 +615,7 @@
         <v>42750</v>
       </c>
       <c r="B16" t="n">
-        <v>1104283.559591549</v>
+        <v>1104035.403920703</v>
       </c>
       <c r="C16" t="n">
         <v>1175725.165838</v>
@@ -626,7 +626,7 @@
         <v>42751</v>
       </c>
       <c r="B17" t="n">
-        <v>1189486.956149474</v>
+        <v>1189229.666963345</v>
       </c>
       <c r="C17" t="n">
         <v>824488.666175</v>
@@ -637,7 +637,7 @@
         <v>42752</v>
       </c>
       <c r="B18" t="n">
-        <v>904434.459687929</v>
+        <v>904163.4886287992</v>
       </c>
       <c r="C18" t="n">
         <v>750836.542952</v>
@@ -648,7 +648,7 @@
         <v>42753</v>
       </c>
       <c r="B19" t="n">
-        <v>904144.6410523052</v>
+        <v>903862.2298358302</v>
       </c>
       <c r="C19" t="n">
         <v>782656.0246723</v>
@@ -659,7 +659,7 @@
         <v>42754</v>
       </c>
       <c r="B20" t="n">
-        <v>936368.7252986624</v>
+        <v>936071.2065589819</v>
       </c>
       <c r="C20" t="n">
         <v>606949.7448793</v>
@@ -670,7 +670,7 @@
         <v>42755</v>
       </c>
       <c r="B21" t="n">
-        <v>926545.6173989382</v>
+        <v>926256.7714669846</v>
       </c>
       <c r="C21" t="n">
         <v>725703.6910875</v>
@@ -681,7 +681,7 @@
         <v>42756</v>
       </c>
       <c r="B22" t="n">
-        <v>1002593.716005552</v>
+        <v>1002285.74715936</v>
       </c>
       <c r="C22" t="n">
         <v>1072721.724905</v>
@@ -692,7 +692,7 @@
         <v>42757</v>
       </c>
       <c r="B23" t="n">
-        <v>1106619.057411964</v>
+        <v>1106284.905098543</v>
       </c>
       <c r="C23" t="n">
         <v>1148214.358454</v>
@@ -703,7 +703,7 @@
         <v>42758</v>
       </c>
       <c r="B24" t="n">
-        <v>1192308.385688315</v>
+        <v>1191968.449857121</v>
       </c>
       <c r="C24" t="n">
         <v>798133.612125</v>
@@ -714,7 +714,7 @@
         <v>42759</v>
       </c>
       <c r="B25" t="n">
-        <v>907636.2891775591</v>
+        <v>907285.5084441648</v>
       </c>
       <c r="C25" t="n">
         <v>721275.774781</v>
@@ -725,7 +725,7 @@
         <v>42760</v>
       </c>
       <c r="B26" t="n">
-        <v>907644.1575474866</v>
+        <v>907284.3224335102</v>
       </c>
       <c r="C26" t="n">
         <v>744342.5929227</v>
@@ -736,7 +736,7 @@
         <v>42761</v>
       </c>
       <c r="B27" t="n">
-        <v>940101.1612302719</v>
+        <v>939728.2153582976</v>
       </c>
       <c r="C27" t="n">
         <v>576515.5369877</v>
@@ -747,7 +747,7 @@
         <v>42762</v>
       </c>
       <c r="B28" t="n">
-        <v>930460.3228040917</v>
+        <v>930097.7145033354</v>
       </c>
       <c r="C28" t="n">
         <v>722113.958837</v>
@@ -758,7 +758,7 @@
         <v>42763</v>
       </c>
       <c r="B29" t="n">
-        <v>1006651.056751198</v>
+        <v>1006270.708171025</v>
       </c>
       <c r="C29" t="n">
         <v>977850.40585</v>
@@ -769,7 +769,7 @@
         <v>42764</v>
       </c>
       <c r="B30" t="n">
-        <v>1110788.012683216</v>
+        <v>1110382.625066747</v>
       </c>
       <c r="C30" t="n">
         <v>1075166.993043</v>
@@ -780,7 +780,7 @@
         <v>42765</v>
       </c>
       <c r="B31" t="n">
-        <v>1196564.681937567</v>
+        <v>1196154.455318861</v>
       </c>
       <c r="C31" t="n">
         <v>698123.768037</v>
@@ -791,7 +791,7 @@
         <v>42766</v>
       </c>
       <c r="B32" t="n">
-        <v>911960.932534982</v>
+        <v>911540.6384695093</v>
       </c>
       <c r="C32" t="n">
         <v>778222.285925</v>
@@ -802,7 +802,7 @@
         <v>42767</v>
       </c>
       <c r="B33" t="n">
-        <v>912022.2844107115</v>
+        <v>911593.5743577761</v>
       </c>
       <c r="C33" t="n">
         <v>961777.382874</v>
@@ -813,7 +813,7 @@
         <v>42768</v>
       </c>
       <c r="B34" t="n">
-        <v>944521.1403447842</v>
+        <v>944079.8425939371</v>
       </c>
       <c r="C34" t="n">
         <v>748882.732615</v>
@@ -824,7 +824,7 @@
         <v>42769</v>
       </c>
       <c r="B35" t="n">
-        <v>934913.0524748609</v>
+        <v>934482.5200055327</v>
       </c>
       <c r="C35" t="n">
         <v>834667.1519293</v>
@@ -835,7 +835,7 @@
         <v>42770</v>
       </c>
       <c r="B36" t="n">
-        <v>1011129.414646645</v>
+        <v>1010681.490999972</v>
       </c>
       <c r="C36" t="n">
         <v>1132788.541413</v>
@@ -846,7 +846,7 @@
         <v>42771</v>
       </c>
       <c r="B37" t="n">
-        <v>1115286.425368011</v>
+        <v>1114813.747146915</v>
       </c>
       <c r="C37" t="n">
         <v>1151987.631095</v>
@@ -857,7 +857,7 @@
         <v>42772</v>
       </c>
       <c r="B38" t="n">
-        <v>1201078.78804822</v>
+        <v>1200601.502256026</v>
       </c>
       <c r="C38" t="n">
         <v>786672.394181</v>
@@ -868,7 +868,7 @@
         <v>42773</v>
       </c>
       <c r="B39" t="n">
-        <v>916487.3191858631</v>
+        <v>916000.1539631831</v>
       </c>
       <c r="C39" t="n">
         <v>739431.213302</v>
@@ -879,7 +879,7 @@
         <v>42774</v>
       </c>
       <c r="B40" t="n">
-        <v>916558.2809235136</v>
+        <v>916062.8522554683</v>
       </c>
       <c r="C40" t="n">
         <v>783605.377185</v>
@@ -890,7 +890,7 @@
         <v>42775</v>
       </c>
       <c r="B41" t="n">
-        <v>949064.6568398473</v>
+        <v>948556.7640813852</v>
       </c>
       <c r="C41" t="n">
         <v>624387.4878990001</v>
@@ -901,7 +901,7 @@
         <v>42776</v>
       </c>
       <c r="B42" t="n">
-        <v>939462.4535638246</v>
+        <v>938965.4261322117</v>
       </c>
       <c r="C42" t="n">
         <v>752207.2398545</v>
@@ -912,7 +912,7 @@
         <v>42777</v>
       </c>
       <c r="B43" t="n">
-        <v>1015683.420592916</v>
+        <v>1015169.082870881</v>
       </c>
       <c r="C43" t="n">
         <v>944924.65301</v>
@@ -923,7 +923,7 @@
         <v>42778</v>
       </c>
       <c r="B44" t="n">
-        <v>1119844.034742322</v>
+        <v>1119305.007776789</v>
       </c>
       <c r="C44" t="n">
         <v>1074820.900014</v>
@@ -934,7 +934,7 @@
         <v>42779</v>
       </c>
       <c r="B45" t="n">
-        <v>1205639.217204515</v>
+        <v>1205095.635384208</v>
       </c>
       <c r="C45" t="n">
         <v>794314.4320675</v>
@@ -945,7 +945,7 @@
         <v>42780</v>
       </c>
       <c r="B46" t="n">
-        <v>921049.9548994583</v>
+        <v>920496.5361479605</v>
       </c>
       <c r="C46" t="n">
         <v>642613.187069</v>
@@ -956,7 +956,7 @@
         <v>42781</v>
       </c>
       <c r="B47" t="n">
-        <v>921122.6433291518</v>
+        <v>920560.9953657604</v>
       </c>
       <c r="C47" t="n">
         <v>745780.355084</v>
@@ -967,7 +967,7 @@
         <v>42782</v>
       </c>
       <c r="B48" t="n">
-        <v>953630.3704297082</v>
+        <v>953056.2859291778</v>
       </c>
       <c r="C48" t="n">
         <v>645968.2570671</v>
@@ -978,7 +978,7 @@
         <v>42783</v>
       </c>
       <c r="B49" t="n">
-        <v>944029.2244926661</v>
+        <v>943466.0274788699</v>
       </c>
       <c r="C49" t="n">
         <v>758855.71279</v>
@@ -989,7 +989,7 @@
         <v>42784</v>
       </c>
       <c r="B50" t="n">
-        <v>1020251.018918719</v>
+        <v>1019670.52942397</v>
       </c>
       <c r="C50" t="n">
         <v>1063394.844003</v>
@@ -1000,7 +1000,7 @@
         <v>42785</v>
       </c>
       <c r="B51" t="n">
-        <v>1124412.280529103</v>
+        <v>1123807.116094268</v>
       </c>
       <c r="C51" t="n">
         <v>858897.1230135</v>
@@ -1011,7 +1011,7 @@
         <v>42786</v>
       </c>
       <c r="B52" t="n">
-        <v>1210207.969647398</v>
+        <v>1209598.26183796</v>
       </c>
       <c r="C52" t="n">
         <v>759120.0599607</v>
@@ -1022,7 +1022,7 @@
         <v>42787</v>
       </c>
       <c r="B53" t="n">
-        <v>925619.1038147371</v>
+        <v>924999.5682826475</v>
       </c>
       <c r="C53" t="n">
         <v>717807.6770255</v>
@@ -1033,7 +1033,7 @@
         <v>42788</v>
       </c>
       <c r="B54" t="n">
-        <v>925692.1024950328</v>
+        <v>925064.3451331435</v>
       </c>
       <c r="C54" t="n">
         <v>739388.0344027</v>
@@ -1044,7 +1044,7 @@
         <v>42789</v>
       </c>
       <c r="B55" t="n">
-        <v>958200.072375256</v>
+        <v>957559.8843908444</v>
       </c>
       <c r="C55" t="n">
         <v>675578.500156</v>
@@ -1055,7 +1055,7 @@
         <v>42790</v>
       </c>
       <c r="B56" t="n">
-        <v>948599.11642001</v>
+        <v>947969.8206586731</v>
       </c>
       <c r="C56" t="n">
         <v>816197.4989520001</v>
@@ -1066,7 +1066,7 @@
         <v>42791</v>
       </c>
       <c r="B57" t="n">
-        <v>1024821.059512066</v>
+        <v>1024174.475060646</v>
       </c>
       <c r="C57" t="n">
         <v>1026011.2228075</v>
@@ -1077,7 +1077,7 @@
         <v>42792</v>
       </c>
       <c r="B58" t="n">
-        <v>1128982.437457705</v>
+        <v>1128311.181098859</v>
       </c>
       <c r="C58" t="n">
         <v>775708.987978</v>
@@ -1088,7 +1088,7 @@
         <v>42793</v>
       </c>
       <c r="B59" t="n">
-        <v>1214778.21761155</v>
+        <v>1214102.420303075</v>
       </c>
       <c r="C59" t="n">
         <v>744956.948138</v>
@@ -1099,7 +1099,7 @@
         <v>42794</v>
       </c>
       <c r="B60" t="n">
-        <v>930189.4230167229</v>
+        <v>929503.7999237874</v>
       </c>
       <c r="C60" t="n">
         <v>949366.8290504999</v>
@@ -1110,7 +1110,7 @@
         <v>42795</v>
       </c>
       <c r="B61" t="n">
-        <v>930262.477442591</v>
+        <v>929568.6340683191</v>
       </c>
       <c r="C61" t="n">
         <v>1008521.709962</v>
@@ -1121,7 +1121,7 @@
         <v>42796</v>
       </c>
       <c r="B62" t="n">
-        <v>962770.4909452645</v>
+        <v>962064.2181850644</v>
       </c>
       <c r="C62" t="n">
         <v>836225.179072</v>
@@ -1132,7 +1132,7 @@
         <v>42797</v>
       </c>
       <c r="B63" t="n">
-        <v>953169.569125791</v>
+        <v>952474.1895758135</v>
       </c>
       <c r="C63" t="n">
         <v>882639.7762739999</v>
@@ -1143,7 +1143,7 @@
         <v>42798</v>
       </c>
       <c r="B64" t="n">
-        <v>1029391.538930032</v>
+        <v>1028678.871477693</v>
       </c>
       <c r="C64" t="n">
         <v>1125736.3470592</v>
@@ -1154,7 +1154,7 @@
         <v>42799</v>
       </c>
       <c r="B65" t="n">
-        <v>1133552.937778694</v>
+        <v>1132815.599047284</v>
       </c>
       <c r="C65" t="n">
         <v>1196983.690104</v>
@@ -1165,7 +1165,7 @@
         <v>42800</v>
       </c>
       <c r="B66" t="n">
-        <v>1219348.734289732</v>
+        <v>1218606.855109747</v>
       </c>
       <c r="C66" t="n">
         <v>790143.2410905</v>
@@ -1176,7 +1176,7 @@
         <v>42801</v>
       </c>
       <c r="B67" t="n">
-        <v>934759.9524948591</v>
+        <v>934008.2479298246</v>
       </c>
       <c r="C67" t="n">
         <v>761866.729975</v>
@@ -1187,7 +1187,7 @@
         <v>42802</v>
       </c>
       <c r="B68" t="n">
-        <v>934833.0169370457</v>
+        <v>934073.0924089553</v>
       </c>
       <c r="C68" t="n">
         <v>781046.6619577</v>
@@ -1198,7 +1198,7 @@
         <v>42803</v>
       </c>
       <c r="B69" t="n">
-        <v>967341.038277765</v>
+        <v>966568.6846172974</v>
       </c>
       <c r="C69" t="n">
         <v>653901.1919827</v>
@@ -1209,7 +1209,7 @@
         <v>42804</v>
       </c>
       <c r="B70" t="n">
-        <v>957740.122591779</v>
+        <v>956978.662343458</v>
       </c>
       <c r="C70" t="n">
         <v>773855.3068500001</v>
@@ -1220,7 +1220,7 @@
         <v>42805</v>
       </c>
       <c r="B71" t="n">
-        <v>1033962.097195644</v>
+        <v>1033183.349205723</v>
       </c>
       <c r="C71" t="n">
         <v>1001174.4340065</v>
@@ -1231,7 +1231,7 @@
         <v>42806</v>
       </c>
       <c r="B72" t="n">
-        <v>1138123.499800143</v>
+        <v>1137320.080659107</v>
       </c>
       <c r="C72" t="n">
         <v>1146006.826973</v>
@@ -1242,7 +1242,7 @@
         <v>42807</v>
       </c>
       <c r="B73" t="n">
-        <v>1223919.299250228</v>
+        <v>1223111.339762432</v>
       </c>
       <c r="C73" t="n">
         <v>754390.380036</v>
@@ -1253,7 +1253,7 @@
         <v>42808</v>
       </c>
       <c r="B74" t="n">
-        <v>939330.5197552406</v>
+        <v>938512.7349633875</v>
       </c>
       <c r="C74" t="n">
         <v>700998.0346447</v>
@@ -1264,7 +1264,7 @@
         <v>42809</v>
       </c>
       <c r="B75" t="n">
-        <v>939403.5859971511</v>
+        <v>938577.5813066553</v>
       </c>
       <c r="C75" t="n">
         <v>815621.887369</v>
@@ -1275,7 +1275,7 @@
         <v>42810</v>
       </c>
       <c r="B76" t="n">
-        <v>971911.6087462041</v>
+        <v>971073.1749745456</v>
       </c>
       <c r="C76" t="n">
         <v>699108.166824</v>
@@ -1286,7 +1286,7 @@
         <v>42811</v>
       </c>
       <c r="B77" t="n">
-        <v>962310.694162278</v>
+        <v>961483.1538434768</v>
       </c>
       <c r="C77" t="n">
         <v>812306.7742700001</v>
@@ -1297,7 +1297,7 @@
         <v>42812</v>
       </c>
       <c r="B78" t="n">
-        <v>1038532.669628535</v>
+        <v>1037687.841600487</v>
       </c>
       <c r="C78" t="n">
         <v>1038906.566154</v>
@@ -1308,7 +1308,7 @@
         <v>42813</v>
       </c>
       <c r="B79" t="n">
-        <v>1142694.07290788</v>
+        <v>1141824.573754423</v>
       </c>
       <c r="C79" t="n">
         <v>1157140.638587</v>
@@ -1319,7 +1319,7 @@
         <v>42814</v>
       </c>
       <c r="B80" t="n">
-        <v>1228489.87288605</v>
+        <v>1227615.833406253</v>
       </c>
       <c r="C80" t="n">
         <v>826428.90991</v>
@@ -1330,7 +1330,7 @@
         <v>42815</v>
       </c>
       <c r="B81" t="n">
-        <v>943901.0938043048</v>
+        <v>943017.2290366678</v>
       </c>
       <c r="C81" t="n">
         <v>746620.926177</v>
@@ -1341,7 +1341,7 @@
         <v>42816</v>
       </c>
       <c r="B82" t="n">
-        <v>943974.1603695882</v>
+        <v>943082.0757161855</v>
       </c>
       <c r="C82" t="n">
         <v>767880.804934</v>
@@ -1352,7 +1352,7 @@
         <v>42817</v>
       </c>
       <c r="B83" t="n">
-        <v>976482.1833716894</v>
+        <v>975577.6696473466</v>
       </c>
       <c r="C83" t="n">
         <v>670848.010029</v>
@@ -1363,7 +1363,7 @@
         <v>42818</v>
       </c>
       <c r="B84" t="n">
-        <v>966881.2689857805</v>
+        <v>965987.6487224088</v>
       </c>
       <c r="C84" t="n">
         <v>787914.125515</v>
@@ -1374,7 +1374,7 @@
         <v>42819</v>
       </c>
       <c r="B85" t="n">
-        <v>1043103.244606992</v>
+        <v>1042192.336640812</v>
       </c>
       <c r="C85" t="n">
         <v>1038139.316887</v>
@@ -1385,7 +1385,7 @@
         <v>42820</v>
       </c>
       <c r="B86" t="n">
-        <v>1147264.648007592</v>
+        <v>1146329.068921112</v>
       </c>
       <c r="C86" t="n">
         <v>1101557.476706</v>
@@ -1396,7 +1396,7 @@
         <v>42821</v>
       </c>
       <c r="B87" t="n">
-        <v>1233060.448080649</v>
+        <v>1232120.328671881</v>
       </c>
       <c r="C87" t="n">
         <v>784103.265042</v>
@@ -1407,7 +1407,7 @@
         <v>42822</v>
       </c>
       <c r="B88" t="n">
-        <v>948471.669073154</v>
+        <v>947521.7243797603</v>
       </c>
       <c r="C88" t="n">
         <v>702943.9485770001</v>
@@ -1418,7 +1418,7 @@
         <v>42823</v>
       </c>
       <c r="B89" t="n">
-        <v>948544.7356965407</v>
+        <v>947586.5711199301</v>
       </c>
       <c r="C89" t="n">
         <v>824632.985033</v>
@@ -1429,7 +1429,7 @@
         <v>42824</v>
       </c>
       <c r="B90" t="n">
-        <v>981052.7587441094</v>
+        <v>980082.1650985796</v>
       </c>
       <c r="C90" t="n">
         <v>637624.340998</v>
@@ -1440,7 +1440,7 @@
         <v>42825</v>
       </c>
       <c r="B91" t="n">
-        <v>971451.8443937801</v>
+        <v>970492.1442108233</v>
       </c>
       <c r="C91" t="n">
         <v>878750.03788</v>
@@ -1451,7 +1451,7 @@
         <v>42826</v>
       </c>
       <c r="B92" t="n">
-        <v>1047673.820042833</v>
+        <v>1046696.832158338</v>
       </c>
       <c r="C92" t="n">
         <v>1463083.962459</v>
@@ -1462,7 +1462,7 @@
         <v>42827</v>
       </c>
       <c r="B93" t="n">
-        <v>1151835.223465221</v>
+        <v>1150833.564461432</v>
       </c>
       <c r="C93" t="n">
         <v>1138650.058898</v>
@@ -1473,7 +1473,7 @@
         <v>42828</v>
       </c>
       <c r="B94" t="n">
-        <v>1237631.023555327</v>
+        <v>1236624.824230047</v>
       </c>
       <c r="C94" t="n">
         <v>835191.622029</v>
@@ -1484,7 +1484,7 @@
         <v>42829</v>
       </c>
       <c r="B95" t="n">
-        <v>953042.244561173</v>
+        <v>952026.2199518993</v>
       </c>
       <c r="C95" t="n">
         <v>835602.6360017</v>
@@ -1495,7 +1495,7 @@
         <v>42830</v>
       </c>
       <c r="B96" t="n">
-        <v>953115.3111949997</v>
+        <v>952091.0667030094</v>
       </c>
       <c r="C96" t="n">
         <v>846631.307907</v>
@@ -1506,7 +1506,7 @@
         <v>42831</v>
       </c>
       <c r="B97" t="n">
-        <v>985623.334250738</v>
+        <v>984586.6606902247</v>
       </c>
       <c r="C97" t="n">
         <v>683059.570103</v>
@@ -1517,7 +1517,7 @@
         <v>42832</v>
       </c>
       <c r="B98" t="n">
-        <v>976022.4199068017</v>
+        <v>974996.6398091753</v>
       </c>
       <c r="C98" t="n">
         <v>765502.211925</v>
@@ -1528,7 +1528,7 @@
         <v>42833</v>
       </c>
       <c r="B99" t="n">
-        <v>1052244.395560857</v>
+        <v>1051201.327761941</v>
       </c>
       <c r="C99" t="n">
         <v>988591.469958</v>
@@ -1539,7 +1539,7 @@
         <v>42834</v>
       </c>
       <c r="B100" t="n">
-        <v>1156405.79898716</v>
+        <v>1155338.060069146</v>
       </c>
       <c r="C100" t="n">
         <v>1101713.657101</v>
@@ -1550,7 +1550,7 @@
         <v>42835</v>
       </c>
       <c r="B101" t="n">
-        <v>1242201.599080329</v>
+        <v>1241129.31984098</v>
       </c>
       <c r="C101" t="n">
         <v>739392.130988</v>
@@ -1561,7 +1561,7 @@
         <v>42836</v>
       </c>
       <c r="B102" t="n">
-        <v>957612.8200885723</v>
+        <v>956530.7155653533</v>
       </c>
       <c r="C102" t="n">
         <v>741331.430196</v>
@@ -1572,7 +1572,7 @@
         <v>42837</v>
       </c>
       <c r="B103" t="n">
-        <v>957685.886724275</v>
+        <v>956595.5623184368</v>
       </c>
       <c r="C103" t="n">
         <v>791762.312883</v>
@@ -1583,7 +1583,7 @@
         <v>42838</v>
       </c>
       <c r="B104" t="n">
-        <v>990193.9097814811</v>
+        <v>989091.1563071972</v>
       </c>
       <c r="C104" t="n">
         <v>737029.5651830001</v>
@@ -1594,7 +1594,7 @@
         <v>42839</v>
       </c>
       <c r="B105" t="n">
-        <v>980592.9954386934</v>
+        <v>979501.1354273575</v>
       </c>
       <c r="C105" t="n">
         <v>740889.4868289999</v>
@@ -1605,7 +1605,7 @@
         <v>42840</v>
       </c>
       <c r="B106" t="n">
-        <v>1056814.971093648</v>
+        <v>1055705.823381071</v>
       </c>
       <c r="C106" t="n">
         <v>898610.217928</v>
@@ -1616,7 +1616,7 @@
         <v>42841</v>
       </c>
       <c r="B107" t="n">
-        <v>1160976.374520654</v>
+        <v>1159842.555689017</v>
       </c>
       <c r="C107" t="n">
         <v>985493.795113</v>
@@ -1627,7 +1627,7 @@
         <v>42842</v>
       </c>
       <c r="B108" t="n">
-        <v>1246772.174614373</v>
+        <v>1245633.815461432</v>
       </c>
       <c r="C108" t="n">
         <v>775916.9059055001</v>
@@ -1638,7 +1638,7 @@
         <v>42843</v>
       </c>
       <c r="B109" t="n">
-        <v>962183.3956230475</v>
+        <v>961035.2111862596</v>
       </c>
       <c r="C109" t="n">
         <v>717196.315762</v>
@@ -1649,7 +1649,7 @@
         <v>42844</v>
       </c>
       <c r="B110" t="n">
-        <v>962256.4622590871</v>
+        <v>961100.057939699</v>
       </c>
       <c r="C110" t="n">
         <v>735733.2142477001</v>
@@ -1660,7 +1660,7 @@
         <v>42845</v>
       </c>
       <c r="B111" t="n">
-        <v>994764.4853165571</v>
+        <v>993595.6519287381</v>
       </c>
       <c r="C111" t="n">
         <v>675804.0219027</v>
@@ -1671,7 +1671,7 @@
         <v>42846</v>
       </c>
       <c r="B112" t="n">
-        <v>985163.5709739758</v>
+        <v>984005.6310491167</v>
       </c>
       <c r="C112" t="n">
         <v>795795.893872</v>
@@ -1682,7 +1682,7 @@
         <v>42847</v>
       </c>
       <c r="B113" t="n">
-        <v>1061385.546629092</v>
+        <v>1060210.319003001</v>
       </c>
       <c r="C113" t="n">
         <v>974952.817869</v>
@@ -1693,7 +1693,7 @@
         <v>42848</v>
       </c>
       <c r="B114" t="n">
-        <v>1165546.950056224</v>
+        <v>1164347.051311081</v>
       </c>
       <c r="C114" t="n">
         <v>1140070.2748035</v>
@@ -1704,7 +1704,7 @@
         <v>42849</v>
       </c>
       <c r="B115" t="n">
-        <v>1251342.750150042</v>
+        <v>1250138.311083601</v>
       </c>
       <c r="C115" t="n">
         <v>755072.530945</v>
@@ -1715,7 +1715,7 @@
         <v>42850</v>
       </c>
       <c r="B116" t="n">
-        <v>966753.971158794</v>
+        <v>965539.7068085102</v>
       </c>
       <c r="C116" t="n">
         <v>718996.080637</v>
@@ -1726,7 +1726,7 @@
         <v>42851</v>
       </c>
       <c r="B117" t="n">
-        <v>966827.0377948942</v>
+        <v>965604.5535620138</v>
       </c>
       <c r="C117" t="n">
         <v>781159.2829995001</v>
@@ -1737,7 +1737,7 @@
         <v>42852</v>
       </c>
       <c r="B118" t="n">
-        <v>999335.0608524116</v>
+        <v>998100.1475511031</v>
       </c>
       <c r="C118" t="n">
         <v>624910.0260955</v>
@@ -1748,7 +1748,7 @@
         <v>42853</v>
       </c>
       <c r="B119" t="n">
-        <v>989734.1465098674</v>
+        <v>988510.1266715211</v>
       </c>
       <c r="C119" t="n">
         <v>797636.6251025</v>
@@ -1759,7 +1759,7 @@
         <v>42854</v>
       </c>
       <c r="B120" t="n">
-        <v>1065956.122165012</v>
+        <v>1064714.814625436</v>
       </c>
       <c r="C120" t="n">
         <v>1068279.815941</v>
@@ -1770,7 +1770,7 @@
         <v>42855</v>
       </c>
       <c r="B121" t="n">
-        <v>1170117.525592168</v>
+        <v>1168851.54693354</v>
       </c>
       <c r="C121" t="n">
         <v>1041249.2479705</v>
@@ -1781,7 +1781,7 @@
         <v>42856</v>
       </c>
       <c r="B122" t="n">
-        <v>1255913.325686003</v>
+        <v>1254642.806706079</v>
       </c>
       <c r="C122" t="n">
         <v>1306699.366897</v>
@@ -1792,7 +1792,7 @@
         <v>42857</v>
       </c>
       <c r="B123" t="n">
-        <v>971324.5466947689</v>
+        <v>970044.2024310032</v>
       </c>
       <c r="C123" t="n">
         <v>907324.094113</v>
@@ -1803,7 +1803,7 @@
         <v>42858</v>
       </c>
       <c r="B124" t="n">
-        <v>971397.6133308801</v>
+        <v>970109.0491845184</v>
       </c>
       <c r="C124" t="n">
         <v>924247.257204</v>
@@ -1814,7 +1814,7 @@
         <v>42859</v>
       </c>
       <c r="B125" t="n">
-        <v>1003905.636388406</v>
+        <v>1002604.643173617</v>
       </c>
       <c r="C125" t="n">
         <v>716654.608983</v>
@@ -1825,7 +1825,7 @@
         <v>42860</v>
       </c>
       <c r="B126" t="n">
-        <v>994304.7220458684</v>
+        <v>993014.6222940419</v>
       </c>
       <c r="C126" t="n">
         <v>780798.407016</v>
@@ -1836,7 +1836,7 @@
         <v>42861</v>
       </c>
       <c r="B127" t="n">
-        <v>1070526.697701019</v>
+        <v>1069219.310247962</v>
       </c>
       <c r="C127" t="n">
         <v>1039417.861868</v>
@@ -1847,7 +1847,7 @@
         <v>42862</v>
       </c>
       <c r="B128" t="n">
-        <v>1174688.101128178</v>
+        <v>1173356.042556071</v>
       </c>
       <c r="C128" t="n">
         <v>1227380.607924</v>
@@ -1858,7 +1858,7 @@
         <v>42863</v>
       </c>
       <c r="B129" t="n">
-        <v>1260483.901222017</v>
+        <v>1259147.302328613</v>
       </c>
       <c r="C129" t="n">
         <v>776307.495015</v>
@@ -1869,7 +1869,7 @@
         <v>42864</v>
       </c>
       <c r="B130" t="n">
-        <v>975895.122230785</v>
+        <v>974548.69805354</v>
       </c>
       <c r="C130" t="n">
         <v>715811.198881</v>
@@ -1880,7 +1880,7 @@
         <v>42865</v>
       </c>
       <c r="B131" t="n">
-        <v>975968.1888668981</v>
+        <v>974613.5448070572</v>
       </c>
       <c r="C131" t="n">
         <v>766101.907094</v>
@@ -1891,7 +1891,7 @@
         <v>42866</v>
       </c>
       <c r="B132" t="n">
-        <v>1008476.211924425</v>
+        <v>1007109.138796157</v>
       </c>
       <c r="C132" t="n">
         <v>648650.413039</v>
@@ -1902,7 +1902,7 @@
         <v>42867</v>
       </c>
       <c r="B133" t="n">
-        <v>998875.2975818891</v>
+        <v>997519.1179165837</v>
       </c>
       <c r="C133" t="n">
         <v>764812.415784</v>
@@ -1913,7 +1913,7 @@
         <v>42868</v>
       </c>
       <c r="B134" t="n">
-        <v>1075097.27323704</v>
+        <v>1073723.805870505</v>
       </c>
       <c r="C134" t="n">
         <v>1116976.891153</v>
@@ -1924,7 +1924,7 @@
         <v>42869</v>
       </c>
       <c r="B135" t="n">
-        <v>1179258.6766642</v>
+        <v>1177860.538178614</v>
       </c>
       <c r="C135" t="n">
         <v>884199.9138385</v>
@@ -1935,7 +1935,7 @@
         <v>42870</v>
       </c>
       <c r="B136" t="n">
-        <v>1265054.47675804</v>
+        <v>1263651.797951157</v>
       </c>
       <c r="C136" t="n">
         <v>823035.572122</v>
@@ -1946,7 +1946,7 @@
         <v>42871</v>
       </c>
       <c r="B137" t="n">
-        <v>980465.6977668083</v>
+        <v>979053.1936760846</v>
       </c>
       <c r="C137" t="n">
         <v>807803.8950783</v>
@@ -1957,7 +1957,7 @@
         <v>42872</v>
       </c>
       <c r="B138" t="n">
-        <v>980538.7644029218</v>
+        <v>979118.0404296023</v>
       </c>
       <c r="C138" t="n">
         <v>841407.607944</v>
@@ -1968,7 +1968,7 @@
         <v>42873</v>
       </c>
       <c r="B139" t="n">
-        <v>1013046.78746045</v>
+        <v>1011613.634418703</v>
       </c>
       <c r="C139" t="n">
         <v>628487.9899620001</v>
@@ -1979,7 +1979,7 @@
         <v>42874</v>
       </c>
       <c r="B140" t="n">
-        <v>1003445.873117913</v>
+        <v>1002023.613539129</v>
       </c>
       <c r="C140" t="n">
         <v>773775.4378677</v>
@@ -1990,7 +1990,7 @@
         <v>42875</v>
       </c>
       <c r="B141" t="n">
-        <v>1079667.848773065</v>
+        <v>1078228.301493051</v>
       </c>
       <c r="C141" t="n">
         <v>1035667.381833</v>
@@ -2001,7 +2001,7 @@
         <v>42876</v>
       </c>
       <c r="B142" t="n">
-        <v>1183829.252200225</v>
+        <v>1182365.03380116</v>
       </c>
       <c r="C142" t="n">
         <v>1201938.886229</v>
@@ -2012,7 +2012,7 @@
         <v>42877</v>
       </c>
       <c r="B143" t="n">
-        <v>1269625.052294065</v>
+        <v>1268156.293573703</v>
       </c>
       <c r="C143" t="n">
         <v>778935.156126</v>
@@ -2023,7 +2023,7 @@
         <v>42878</v>
       </c>
       <c r="B144" t="n">
-        <v>985036.2733028331</v>
+        <v>983557.6892986307</v>
       </c>
       <c r="C144" t="n">
         <v>723151.767982</v>
@@ -2034,7 +2034,7 @@
         <v>42879</v>
       </c>
       <c r="B145" t="n">
-        <v>985109.3399389465</v>
+        <v>983622.5360521484</v>
       </c>
       <c r="C145" t="n">
         <v>746303.6271255</v>
@@ -2045,7 +2045,7 @@
         <v>42880</v>
       </c>
       <c r="B146" t="n">
-        <v>1017617.362996474</v>
+        <v>1016118.130041249</v>
       </c>
       <c r="C146" t="n">
         <v>620108.24391</v>
@@ -2056,7 +2056,7 @@
         <v>42881</v>
       </c>
       <c r="B147" t="n">
-        <v>1008016.448653938</v>
+        <v>1006528.109161675</v>
       </c>
       <c r="C147" t="n">
         <v>984511.1521135001</v>
@@ -2067,7 +2067,7 @@
         <v>42882</v>
       </c>
       <c r="B148" t="n">
-        <v>1084238.42430909</v>
+        <v>1082732.797115597</v>
       </c>
       <c r="C148" t="n">
         <v>932219.893144</v>
@@ -2078,7 +2078,7 @@
         <v>42883</v>
       </c>
       <c r="B149" t="n">
-        <v>1188399.82773625</v>
+        <v>1186869.529423706</v>
       </c>
       <c r="C149" t="n">
         <v>1061771.636907</v>
@@ -2089,7 +2089,7 @@
         <v>42884</v>
       </c>
       <c r="B150" t="n">
-        <v>1274195.62783009</v>
+        <v>1272660.789196249</v>
       </c>
       <c r="C150" t="n">
         <v>776813.137038</v>
@@ -2100,7 +2100,7 @@
         <v>42885</v>
       </c>
       <c r="B151" t="n">
-        <v>989606.8488388581</v>
+        <v>988062.184921177</v>
       </c>
       <c r="C151" t="n">
         <v>742471.2769905</v>
@@ -2111,7 +2111,7 @@
         <v>42886</v>
       </c>
       <c r="B152" t="n">
-        <v>989679.9154749715</v>
+        <v>988127.0316746947</v>
       </c>
       <c r="C152" t="n">
         <v>858062.149411</v>
@@ -2122,7 +2122,7 @@
         <v>42887</v>
       </c>
       <c r="B153" t="n">
-        <v>1022187.938532499</v>
+        <v>1020622.625663795</v>
       </c>
       <c r="C153" t="n">
         <v>766859.1728450001</v>
@@ -2133,7 +2133,7 @@
         <v>42888</v>
       </c>
       <c r="B154" t="n">
-        <v>1012587.024189963</v>
+        <v>1011032.604784222</v>
       </c>
       <c r="C154" t="n">
         <v>918421.319125</v>
@@ -2144,7 +2144,7 @@
         <v>42889</v>
       </c>
       <c r="B155" t="n">
-        <v>1088808.999845115</v>
+        <v>1087237.292738143</v>
       </c>
       <c r="C155" t="n">
         <v>1176138.109152</v>
@@ -2155,7 +2155,7 @@
         <v>42890</v>
       </c>
       <c r="B156" t="n">
-        <v>1192970.403272275</v>
+        <v>1191374.025046253</v>
       </c>
       <c r="C156" t="n">
         <v>1376511.520495</v>
@@ -2166,7 +2166,7 @@
         <v>42891</v>
       </c>
       <c r="B157" t="n">
-        <v>1278766.203366115</v>
+        <v>1277165.284818796</v>
       </c>
       <c r="C157" t="n">
         <v>912693.8511</v>
@@ -2177,7 +2177,7 @@
         <v>42892</v>
       </c>
       <c r="B158" t="n">
-        <v>994177.4243748831</v>
+        <v>992566.6805437234</v>
       </c>
       <c r="C158" t="n">
         <v>805546.6479559999</v>
@@ -2188,7 +2188,7 @@
         <v>42893</v>
       </c>
       <c r="B159" t="n">
-        <v>994250.4910109965</v>
+        <v>992631.5272972411</v>
       </c>
       <c r="C159" t="n">
         <v>842979.8370823</v>
@@ -2199,7 +2199,7 @@
         <v>42894</v>
       </c>
       <c r="B160" t="n">
-        <v>1026758.514068524</v>
+        <v>1025127.121286342</v>
       </c>
       <c r="C160" t="n">
         <v>667099.8010250001</v>
@@ -2210,7 +2210,7 @@
         <v>42895</v>
       </c>
       <c r="B161" t="n">
-        <v>1017157.599725988</v>
+        <v>1015537.100406768</v>
       </c>
       <c r="C161" t="n">
         <v>795116.1360699</v>
@@ -2221,7 +2221,7 @@
         <v>42896</v>
       </c>
       <c r="B162" t="n">
-        <v>1093379.57538114</v>
+        <v>1091741.78836069</v>
       </c>
       <c r="C162" t="n">
         <v>993732.684049</v>
@@ -2232,7 +2232,7 @@
         <v>42897</v>
       </c>
       <c r="B163" t="n">
-        <v>1197540.9788083</v>
+        <v>1195878.520668799</v>
       </c>
       <c r="C163" t="n">
         <v>1213673.946877</v>
@@ -2243,7 +2243,7 @@
         <v>42898</v>
       </c>
       <c r="B164" t="n">
-        <v>1283336.77890214</v>
+        <v>1281669.780441342</v>
       </c>
       <c r="C164" t="n">
         <v>768349.7589516999</v>
@@ -2254,7 +2254,7 @@
         <v>42899</v>
       </c>
       <c r="B165" t="n">
-        <v>998747.9999109081</v>
+        <v>997071.1761662698</v>
       </c>
       <c r="C165" t="n">
         <v>729412.959849</v>
@@ -2265,7 +2265,7 @@
         <v>42900</v>
       </c>
       <c r="B166" t="n">
-        <v>998821.0665470215</v>
+        <v>997136.0229197876</v>
       </c>
       <c r="C166" t="n">
         <v>785885.9088963</v>
@@ -2276,7 +2276,7 @@
         <v>42901</v>
       </c>
       <c r="B167" t="n">
-        <v>1031329.089604549</v>
+        <v>1029631.616908888</v>
       </c>
       <c r="C167" t="n">
         <v>660338.346974</v>
@@ -2287,7 +2287,7 @@
         <v>42902</v>
       </c>
       <c r="B168" t="n">
-        <v>1021728.175262013</v>
+        <v>1020041.596029315</v>
       </c>
       <c r="C168" t="n">
         <v>834786.4275550001</v>
@@ -2298,7 +2298,7 @@
         <v>42903</v>
       </c>
       <c r="B169" t="n">
-        <v>1097950.150917165</v>
+        <v>1096246.283983236</v>
       </c>
       <c r="C169" t="n">
         <v>1096133.5508865</v>
@@ -2309,7 +2309,7 @@
         <v>42904</v>
       </c>
       <c r="B170" t="n">
-        <v>1202111.554344325</v>
+        <v>1200383.016291346</v>
       </c>
       <c r="C170" t="n">
         <v>965144.121179</v>
@@ -2320,7 +2320,7 @@
         <v>42905</v>
       </c>
       <c r="B171" t="n">
-        <v>1287907.354438165</v>
+        <v>1286174.276063889</v>
       </c>
       <c r="C171" t="n">
         <v>791146.393731</v>
@@ -2331,7 +2331,7 @@
         <v>42906</v>
       </c>
       <c r="B172" t="n">
-        <v>1003318.575446933</v>
+        <v>1001575.671788816</v>
       </c>
       <c r="C172" t="n">
         <v>787326.7170395</v>
@@ -2342,7 +2342,7 @@
         <v>42907</v>
       </c>
       <c r="B173" t="n">
-        <v>1003391.642083046</v>
+        <v>1001640.518542334</v>
       </c>
       <c r="C173" t="n">
         <v>766159.0112892</v>
@@ -2353,7 +2353,7 @@
         <v>42908</v>
       </c>
       <c r="B174" t="n">
-        <v>1035899.665140574</v>
+        <v>1034136.112531434</v>
       </c>
       <c r="C174" t="n">
         <v>609868.8309586</v>
@@ -2364,7 +2364,7 @@
         <v>42909</v>
       </c>
       <c r="B175" t="n">
-        <v>1026298.750798038</v>
+        <v>1024546.091651861</v>
       </c>
       <c r="C175" t="n">
         <v>761049.7450639</v>
@@ -2375,7 +2375,7 @@
         <v>42910</v>
       </c>
       <c r="B176" t="n">
-        <v>1102520.72645319</v>
+        <v>1100750.779605783</v>
       </c>
       <c r="C176" t="n">
         <v>963268.2271350001</v>
@@ -2386,7 +2386,7 @@
         <v>42911</v>
       </c>
       <c r="B177" t="n">
-        <v>1206682.12988035</v>
+        <v>1204887.511913892</v>
       </c>
       <c r="C177" t="n">
         <v>1092610.858614</v>
@@ -2397,7 +2397,7 @@
         <v>42912</v>
       </c>
       <c r="B178" t="n">
-        <v>1292477.929974189</v>
+        <v>1290678.771686435</v>
       </c>
       <c r="C178" t="n">
         <v>755367.8450665</v>
@@ -2408,7 +2408,7 @@
         <v>42913</v>
       </c>
       <c r="B179" t="n">
-        <v>1007889.150982958</v>
+        <v>1006080.167411363</v>
       </c>
       <c r="C179" t="n">
         <v>682218.468913</v>
@@ -2419,7 +2419,7 @@
         <v>42914</v>
       </c>
       <c r="B180" t="n">
-        <v>1007962.217619071</v>
+        <v>1006145.01416488</v>
       </c>
       <c r="C180" t="n">
         <v>731896.9850104999</v>
@@ -2430,7 +2430,7 @@
         <v>42915</v>
       </c>
       <c r="B181" t="n">
-        <v>1040470.240676599</v>
+        <v>1038640.608153981</v>
       </c>
       <c r="C181" t="n">
         <v>630811.802872</v>
@@ -2441,7 +2441,7 @@
         <v>42916</v>
       </c>
       <c r="B182" t="n">
-        <v>1030869.326334063</v>
+        <v>1029050.587274408</v>
       </c>
       <c r="C182" t="n">
         <v>802273.1392327</v>
@@ -2452,7 +2452,7 @@
         <v>42917</v>
       </c>
       <c r="B183" t="n">
-        <v>1107091.301989215</v>
+        <v>1105255.275228329</v>
       </c>
       <c r="C183" t="n">
         <v>1207529.921868</v>
@@ -2463,7 +2463,7 @@
         <v>42918</v>
       </c>
       <c r="B184" t="n">
-        <v>1211252.705416375</v>
+        <v>1209392.007536439</v>
       </c>
       <c r="C184" t="n">
         <v>1296379.2175535</v>
@@ -2474,7 +2474,7 @@
         <v>42919</v>
       </c>
       <c r="B185" t="n">
-        <v>1297048.505510214</v>
+        <v>1295183.267308981</v>
       </c>
       <c r="C185" t="n">
         <v>925143.408816</v>
@@ -2485,7 +2485,7 @@
         <v>42920</v>
       </c>
       <c r="B186" t="n">
-        <v>1012459.726518983</v>
+        <v>1010584.663033909</v>
       </c>
       <c r="C186" t="n">
         <v>832359.2860137</v>
@@ -2496,7 +2496,7 @@
         <v>42921</v>
       </c>
       <c r="B187" t="n">
-        <v>1012532.793155096</v>
+        <v>1010649.509787427</v>
       </c>
       <c r="C187" t="n">
         <v>844301.613116</v>
@@ -2507,7 +2507,7 @@
         <v>42922</v>
       </c>
       <c r="B188" t="n">
-        <v>1045040.816212624</v>
+        <v>1043145.103776527</v>
       </c>
       <c r="C188" t="n">
         <v>700272.0099567</v>
@@ -2518,7 +2518,7 @@
         <v>42923</v>
       </c>
       <c r="B189" t="n">
-        <v>1035439.901870088</v>
+        <v>1033555.082896954</v>
       </c>
       <c r="C189" t="n">
         <v>805792.302193</v>
@@ -2529,7 +2529,7 @@
         <v>42924</v>
       </c>
       <c r="B190" t="n">
-        <v>1111661.87752524</v>
+        <v>1109759.770850875</v>
       </c>
       <c r="C190" t="n">
         <v>998347.1930085</v>
@@ -2540,7 +2540,7 @@
         <v>42925</v>
       </c>
       <c r="B191" t="n">
-        <v>1215823.2809524</v>
+        <v>1213896.503158985</v>
       </c>
       <c r="C191" t="n">
         <v>1100833.322376</v>
@@ -2551,7 +2551,7 @@
         <v>42926</v>
       </c>
       <c r="B192" t="n">
-        <v>1301619.081046239</v>
+        <v>1299687.762931528</v>
       </c>
       <c r="C192" t="n">
         <v>804158.8610365</v>
@@ -2562,7 +2562,7 @@
         <v>42927</v>
       </c>
       <c r="B193" t="n">
-        <v>1017030.302055008</v>
+        <v>1015089.158656455</v>
       </c>
       <c r="C193" t="n">
         <v>730534.767701</v>
@@ -2573,7 +2573,7 @@
         <v>42928</v>
       </c>
       <c r="B194" t="n">
-        <v>1017103.368691121</v>
+        <v>1015154.005409973</v>
       </c>
       <c r="C194" t="n">
         <v>748799.9959087</v>
@@ -2584,7 +2584,7 @@
         <v>42929</v>
       </c>
       <c r="B195" t="n">
-        <v>1049611.391748649</v>
+        <v>1047649.599399074</v>
       </c>
       <c r="C195" t="n">
         <v>629651.3629294999</v>
@@ -2595,7 +2595,7 @@
         <v>42930</v>
       </c>
       <c r="B196" t="n">
-        <v>1040010.477406113</v>
+        <v>1038059.5785195</v>
       </c>
       <c r="C196" t="n">
         <v>765489.6173932999</v>
@@ -2606,7 +2606,7 @@
         <v>42931</v>
       </c>
       <c r="B197" t="n">
-        <v>1116232.453061265</v>
+        <v>1114264.266473422</v>
       </c>
       <c r="C197" t="n">
         <v>969077.125075</v>
@@ -2617,7 +2617,7 @@
         <v>42932</v>
       </c>
       <c r="B198" t="n">
-        <v>1220393.856488425</v>
+        <v>1218400.998781531</v>
       </c>
       <c r="C198" t="n">
         <v>1100803.699023</v>
@@ -2628,7 +2628,7 @@
         <v>42933</v>
       </c>
       <c r="B199" t="n">
-        <v>1306189.656582264</v>
+        <v>1304192.258554074</v>
       </c>
       <c r="C199" t="n">
         <v>818325.522149</v>
@@ -2639,7 +2639,7 @@
         <v>42934</v>
       </c>
       <c r="B200" t="n">
-        <v>1021600.877591033</v>
+        <v>1019593.654279002</v>
       </c>
       <c r="C200" t="n">
         <v>730133.70894</v>
@@ -2650,7 +2650,7 @@
         <v>42935</v>
       </c>
       <c r="B201" t="n">
-        <v>1021673.944227146</v>
+        <v>1019658.50103252</v>
       </c>
       <c r="C201" t="n">
         <v>767978.7780779999</v>
@@ -2661,7 +2661,7 @@
         <v>42936</v>
       </c>
       <c r="B202" t="n">
-        <v>1054181.967284674</v>
+        <v>1052154.09502162</v>
       </c>
       <c r="C202" t="n">
         <v>688288.067857</v>
@@ -2672,7 +2672,7 @@
         <v>42937</v>
       </c>
       <c r="B203" t="n">
-        <v>1044581.052942138</v>
+        <v>1042564.074142047</v>
       </c>
       <c r="C203" t="n">
         <v>782418.2992188</v>
@@ -2683,7 +2683,7 @@
         <v>42938</v>
       </c>
       <c r="B204" t="n">
-        <v>1120803.02859729</v>
+        <v>1118768.762095968</v>
       </c>
       <c r="C204" t="n">
         <v>932902.046681</v>
@@ -2694,7 +2694,7 @@
         <v>42939</v>
       </c>
       <c r="B205" t="n">
-        <v>1224964.43202445</v>
+        <v>1222905.494404078</v>
       </c>
       <c r="C205" t="n">
         <v>1024288.741245</v>
@@ -2705,7 +2705,7 @@
         <v>42940</v>
       </c>
       <c r="B206" t="n">
-        <v>1310760.232118289</v>
+        <v>1308696.754176621</v>
       </c>
       <c r="C206" t="n">
         <v>816564.327096</v>
@@ -2716,7 +2716,7 @@
         <v>42941</v>
       </c>
       <c r="B207" t="n">
-        <v>1026171.453127058</v>
+        <v>1024098.149901548</v>
       </c>
       <c r="C207" t="n">
         <v>713581.632609</v>
@@ -2727,7 +2727,7 @@
         <v>42942</v>
       </c>
       <c r="B208" t="n">
-        <v>1026244.519763171</v>
+        <v>1024162.996655066</v>
       </c>
       <c r="C208" t="n">
         <v>740653.044167</v>
@@ -2738,7 +2738,7 @@
         <v>42943</v>
       </c>
       <c r="B209" t="n">
-        <v>1058752.542820699</v>
+        <v>1056658.590644166</v>
       </c>
       <c r="C209" t="n">
         <v>659849.8270588</v>
@@ -2749,7 +2749,7 @@
         <v>42944</v>
       </c>
       <c r="B210" t="n">
-        <v>1049151.628478163</v>
+        <v>1047068.569764593</v>
       </c>
       <c r="C210" t="n">
         <v>835099.6822034999</v>
@@ -2760,7 +2760,7 @@
         <v>42945</v>
       </c>
       <c r="B211" t="n">
-        <v>1125373.604133315</v>
+        <v>1123273.257718515</v>
       </c>
       <c r="C211" t="n">
         <v>1032310.865737</v>
@@ -2771,7 +2771,7 @@
         <v>42946</v>
       </c>
       <c r="B212" t="n">
-        <v>1229535.007560475</v>
+        <v>1227409.990026624</v>
       </c>
       <c r="C212" t="n">
         <v>1123752.4779517</v>
@@ -2782,7 +2782,7 @@
         <v>42947</v>
       </c>
       <c r="B213" t="n">
-        <v>1315330.807654314</v>
+        <v>1313201.249799167</v>
       </c>
       <c r="C213" t="n">
         <v>885856.8408705</v>
@@ -2793,7 +2793,7 @@
         <v>42948</v>
       </c>
       <c r="B214" t="n">
-        <v>1030742.028663083</v>
+        <v>1028602.645524095</v>
       </c>
       <c r="C214" t="n">
         <v>988527.763204</v>
@@ -2804,7 +2804,7 @@
         <v>42949</v>
       </c>
       <c r="B215" t="n">
-        <v>1030815.095299196</v>
+        <v>1028667.492277612</v>
       </c>
       <c r="C215" t="n">
         <v>964712.016051</v>
@@ -2815,7 +2815,7 @@
         <v>42950</v>
       </c>
       <c r="B216" t="n">
-        <v>1063323.118356724</v>
+        <v>1061163.086266713</v>
       </c>
       <c r="C216" t="n">
         <v>728068.4851319999</v>
@@ -2826,7 +2826,7 @@
         <v>42951</v>
       </c>
       <c r="B217" t="n">
-        <v>1053722.204014188</v>
+        <v>1051573.06538714</v>
       </c>
       <c r="C217" t="n">
         <v>827775.686128</v>
@@ -2837,7 +2837,7 @@
         <v>42952</v>
       </c>
       <c r="B218" t="n">
-        <v>1129944.17966934</v>
+        <v>1127777.753341061</v>
       </c>
       <c r="C218" t="n">
         <v>965693.650492</v>
@@ -2848,7 +2848,7 @@
         <v>42953</v>
       </c>
       <c r="B219" t="n">
-        <v>1234105.5830965</v>
+        <v>1231914.485649171</v>
       </c>
       <c r="C219" t="n">
         <v>1049559.164277</v>
@@ -2859,7 +2859,7 @@
         <v>42954</v>
       </c>
       <c r="B220" t="n">
-        <v>1319901.383190339</v>
+        <v>1317705.745421713</v>
       </c>
       <c r="C220" t="n">
         <v>797464.963817</v>
@@ -2870,7 +2870,7 @@
         <v>42955</v>
       </c>
       <c r="B221" t="n">
-        <v>1035312.604199108</v>
+        <v>1033107.141146641</v>
       </c>
       <c r="C221" t="n">
         <v>717766.3491055</v>
@@ -2881,7 +2881,7 @@
         <v>42956</v>
       </c>
       <c r="B222" t="n">
-        <v>1035385.670835221</v>
+        <v>1033171.987900159</v>
       </c>
       <c r="C222" t="n">
         <v>734139.67401</v>
@@ -2892,7 +2892,7 @@
         <v>42957</v>
       </c>
       <c r="B223" t="n">
-        <v>1067893.693892749</v>
+        <v>1065667.581889259</v>
       </c>
       <c r="C223" t="n">
         <v>651386.9119697</v>
@@ -2903,7 +2903,7 @@
         <v>42958</v>
       </c>
       <c r="B224" t="n">
-        <v>1058292.779550213</v>
+        <v>1056077.561009686</v>
       </c>
       <c r="C224" t="n">
         <v>826373.722022</v>
@@ -2914,7 +2914,7 @@
         <v>42959</v>
       </c>
       <c r="B225" t="n">
-        <v>1134514.755205365</v>
+        <v>1132282.248963607</v>
       </c>
       <c r="C225" t="n">
         <v>792630.5350785</v>
@@ -2925,7 +2925,7 @@
         <v>42960</v>
       </c>
       <c r="B226" t="n">
-        <v>1238676.158632525</v>
+        <v>1236418.981271717</v>
       </c>
       <c r="C226" t="n">
         <v>865639.677471</v>
@@ -2936,7 +2936,7 @@
         <v>42961</v>
       </c>
       <c r="B227" t="n">
-        <v>1324471.958726364</v>
+        <v>1322210.24104426</v>
       </c>
       <c r="C227" t="n">
         <v>760922.4060808</v>
@@ -2947,7 +2947,7 @@
         <v>42962</v>
       </c>
       <c r="B228" t="n">
-        <v>1039883.179735133</v>
+        <v>1037611.636769188</v>
       </c>
       <c r="C228" t="n">
         <v>762661.935939</v>

</xml_diff>